<commit_message>
LOE updates for August
</commit_message>
<xml_diff>
--- a/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
+++ b/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
@@ -24,7 +24,7 @@
     <sheet name="Support" sheetId="8" state="hidden" r:id="rId15"/>
     <sheet name="SB-Manager" sheetId="26" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -374,15 +374,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -565,7 +558,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="105">
@@ -707,21 +700,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -736,7 +729,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1136,11 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1318,7 +1310,9 @@
       <c r="G6" s="3">
         <v>16</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3">
+        <v>12</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1331,11 +1325,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="40">
         <f>SUM(G6:R6)</f>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="U6" s="4">
         <f>T6/MAX(C6,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -1359,7 +1353,9 @@
       <c r="G7" s="3">
         <v>8</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <v>8</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1372,11 +1368,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="40">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U7" s="4">
         <f>T7/MAX(C7,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1629,7 +1625,9 @@
       <c r="G14" s="3">
         <v>4</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <v>8</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1642,11 +1640,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="40">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1784,7 +1782,7 @@
       </c>
       <c r="H18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I18" s="79">
         <f t="shared" si="2"/>
@@ -1828,11 +1826,11 @@
       </c>
       <c r="T18" s="40">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="1"/>
-        <v>7.2916666666666671E-2</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -1849,7 +1847,7 @@
       </c>
       <c r="H19" s="4">
         <f xml:space="preserve"> IF(H18=0, 0,(H18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="I19" s="4">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-F18)/F18)</f>
@@ -1907,7 +1905,7 @@
       </c>
       <c r="H21" s="80">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="I21" s="80">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -1957,7 +1955,7 @@
       </c>
       <c r="H22" s="40">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>328</v>
       </c>
       <c r="I22" s="40">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -2007,7 +2005,7 @@
       </c>
       <c r="H23" s="40">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="40">
         <f ca="1">'Project Summary'!I16</f>
@@ -2051,7 +2049,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -2071,11 +2068,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2286,7 +2282,9 @@
       <c r="G7" s="14">
         <v>8</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14">
+        <v>8</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -2299,11 +2297,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2705,7 +2703,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -2749,11 +2747,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="28" hidden="1">
@@ -2828,7 +2826,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -2878,7 +2876,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -2928,7 +2926,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -2972,7 +2970,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -2991,11 +2988,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3205,7 +3201,9 @@
       <c r="G7" s="14">
         <v>11</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14">
+        <v>12</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -3218,11 +3216,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>8.59375E-2</v>
+        <v>0.1796875</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3475,7 +3473,9 @@
       <c r="G14" s="14">
         <v>5</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14">
+        <v>4</v>
+      </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -3488,11 +3488,11 @@
       <c r="R14" s="14"/>
       <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
+        <v>0.140625</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3515,7 +3515,9 @@
       <c r="G15" s="14">
         <v>6</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>6</v>
+      </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -3528,11 +3530,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>9.375E-2</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3555,7 +3557,9 @@
       <c r="G16" s="14">
         <v>6</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="14">
+        <v>6</v>
+      </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -3568,11 +3572,11 @@
       <c r="R16" s="14"/>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="1"/>
-        <v>9.375E-2</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3595,7 +3599,9 @@
       <c r="G17" s="14">
         <v>5</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14">
+        <v>5</v>
+      </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
@@ -3608,11 +3614,11 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>7.8125E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
@@ -3636,7 +3642,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -3680,11 +3686,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -3701,7 +3707,7 @@
       </c>
       <c r="H19" s="26">
         <f xml:space="preserve"> IF(H18=0, 0,(H18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I19" s="26">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-F18)/F18)</f>
@@ -3756,7 +3762,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -3806,7 +3812,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>352</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -3856,7 +3862,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -3900,7 +3906,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -3922,11 +3927,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4289,7 +4293,9 @@
         <v>40344</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+      <c r="H11" s="14">
+        <v>160</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
@@ -4302,11 +4308,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -4558,7 +4564,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -4602,11 +4608,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>260</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>5.2083333333333336E-2</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -4678,7 +4684,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -4728,7 +4734,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>1660</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -4778,7 +4784,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -4822,7 +4828,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -4841,7 +4846,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
@@ -5017,7 +5021,7 @@
       </c>
       <c r="H4" s="43">
         <f>Warren!H18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I4" s="43">
         <f>Warren!I18</f>
@@ -5061,11 +5065,11 @@
       </c>
       <c r="S4" s="88">
         <f t="shared" ref="S4:S15" si="0">SUM(G4:R4)</f>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="T4" s="28">
         <f>S4/MAX(1,D4)</f>
-        <v>7.2916666666666671E-2</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5098,7 +5102,7 @@
       </c>
       <c r="H5" s="43">
         <f>Sean!H18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I5" s="43">
         <f>Sean!I18</f>
@@ -5142,11 +5146,11 @@
       </c>
       <c r="S5" s="88">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ref="T5:T16" si="1">S5/MAX(1,D5)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5179,7 +5183,7 @@
       </c>
       <c r="H6" s="43">
         <f>Rhett!H18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="I6" s="43">
         <f>Rhett!I18</f>
@@ -5223,11 +5227,11 @@
       </c>
       <c r="S6" s="88">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5260,7 +5264,7 @@
       </c>
       <c r="H7" s="43">
         <f>Jalpa!H18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I7" s="43">
         <f ca="1">Warren!I21</f>
@@ -5341,7 +5345,7 @@
       </c>
       <c r="H8" s="43">
         <f>Nataliya!H18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I8" s="43">
         <f>Nataliya!I18</f>
@@ -5385,11 +5389,11 @@
       </c>
       <c r="S8" s="88">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5422,7 +5426,7 @@
       </c>
       <c r="H9" s="43">
         <f>John!H18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I9" s="43">
         <f>John!I18</f>
@@ -5503,7 +5507,7 @@
       </c>
       <c r="H10" s="43">
         <f>David!H18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I10" s="43">
         <f>David!I18</f>
@@ -5547,11 +5551,11 @@
       </c>
       <c r="S10" s="88">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>7.7083333333333337E-2</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="40" customFormat="1">
@@ -5665,7 +5669,7 @@
       </c>
       <c r="H12" s="43">
         <f>Renee!H18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I12" s="43">
         <f>Renee!I18</f>
@@ -5709,11 +5713,11 @@
       </c>
       <c r="S12" s="88">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5746,7 +5750,7 @@
       </c>
       <c r="H13" s="43">
         <f>Dong!H18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I13" s="43">
         <f>Dong!I18</f>
@@ -5790,11 +5794,11 @@
       </c>
       <c r="S13" s="88">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5827,7 +5831,7 @@
       </c>
       <c r="H14" s="43">
         <f>Lee!H18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I14" s="43">
         <f>Lee!I18</f>
@@ -5871,11 +5875,11 @@
       </c>
       <c r="S14" s="88">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -5908,7 +5912,7 @@
       </c>
       <c r="H15" s="84">
         <f>'SB-Dev'!H18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I15" s="84">
         <f>'SB-Dev'!I18</f>
@@ -5952,11 +5956,11 @@
       </c>
       <c r="S15" s="88">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>260</v>
       </c>
       <c r="T15" s="28">
         <f t="shared" si="1"/>
-        <v>5.2083333333333336E-2</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1">
@@ -5977,7 +5981,7 @@
       </c>
       <c r="H16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" ca="1" si="2"/>
@@ -6101,7 +6105,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -6123,7 +6126,6 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -6308,7 +6310,7 @@
       </c>
       <c r="H6" s="14">
         <f>Warren!H6+Sean!H6+Rhett!H6+Jalpa!H6+Nataliya!H6+John!H6+Renee!H6+Dong!H6+Lee!H6</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="I6" s="14">
         <f>Warren!I6+Sean!I6+Rhett!I6+Jalpa!I6+Nataliya!I6+John!I6+Renee!I6+Dong!I6+Lee!I6</f>
@@ -6352,11 +6354,11 @@
       </c>
       <c r="T6">
         <f>SUM(G6:R6)</f>
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" ref="U6:U18" si="0">T6/MAX(1,D6)</f>
-        <v>9.8214285714285712E-2</v>
+        <v>0.19047619047619047</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6385,7 +6387,7 @@
       </c>
       <c r="H7" s="14">
         <f>Warren!H7+Sean!H7+Rhett!H7+Jalpa!H7+Nataliya!H7+John!H7+Renee!H7+Dong!H7+Lee!H7</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I7" s="14">
         <f>Warren!I7+Sean!I7+Rhett!I7+Jalpa!I7+Nataliya!I7+John!I7+Renee!I7+Dong!I7+Lee!I7</f>
@@ -6429,11 +6431,11 @@
       </c>
       <c r="T7">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>78</v>
+        <v>120</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>8.5526315789473686E-2</v>
+        <v>0.13157894736842105</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6462,7 +6464,7 @@
       </c>
       <c r="H8" s="14">
         <f>Warren!H8+Sean!H8+Rhett!H8+Jalpa!H8+Nataliya!H8+John!H8+Renee!H8+Dong!H8+Lee!H8</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I8" s="14">
         <f>Warren!I8+Sean!I8+Rhett!I8+Jalpa!I8+Nataliya!I8+John!I8+Renee!I8+Dong!I8+Lee!I8</f>
@@ -6506,11 +6508,11 @@
       </c>
       <c r="T8">
         <f t="shared" si="1"/>
-        <v>570</v>
+        <v>650</v>
       </c>
       <c r="U8" s="11">
         <f t="shared" si="0"/>
-        <v>6.7471590909090912E-2</v>
+        <v>7.6941287878787873E-2</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -6616,7 +6618,7 @@
       </c>
       <c r="H10" s="14">
         <f>Warren!H10+Sean!H10+Rhett!H10+Jalpa!H10+Nataliya!H10+John!H10+Renee!H10+Dong!H10+Lee!H10</f>
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="I10" s="14">
         <f>Warren!I10+Sean!I10+Rhett!I10+Jalpa!I10+Nataliya!I10+John!I10+Renee!I10+Dong!I10+Lee!I10</f>
@@ -6660,11 +6662,11 @@
       </c>
       <c r="T10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>368</v>
       </c>
       <c r="U10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6770,7 +6772,7 @@
       </c>
       <c r="H12" s="14">
         <f>Warren!H12+Sean!H12+Rhett!H12+Jalpa!H12+Nataliya!H12+John!H12+Renee!H12+Dong!H12+Lee!H12</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I12" s="14">
         <f>Warren!I12+Sean!I12+Rhett!I12+Jalpa!I12+Nataliya!I12+John!I12+Renee!I12+Dong!I12+Lee!I12</f>
@@ -6814,11 +6816,11 @@
       </c>
       <c r="T12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6846,7 +6848,7 @@
       </c>
       <c r="H13" s="14">
         <f>Warren!H13+Sean!H13+Rhett!H13+Jalpa!H13+Nataliya!H13+John!H13+Renee!H13+Dong!H13+Lee!H13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="I13" s="14">
         <f>Warren!I13+Sean!I13+Rhett!I13+Jalpa!I13+Nataliya!I13+John!I13+Renee!I13+Dong!I13+Lee!I13</f>
@@ -6890,11 +6892,11 @@
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="U13" s="11">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>1.8333333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28">
@@ -6922,7 +6924,7 @@
       </c>
       <c r="H14" s="14">
         <f>Warren!H14+Sean!H14+Rhett!H14+Jalpa!H14+Nataliya!H14+John!H14+Renee!H14+Dong!H14+Lee!H14</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I14" s="14">
         <f>Warren!I14+Sean!I14+Rhett!I14+Jalpa!I14+Nataliya!I14+John!I14+Renee!I14+Dong!I14+Lee!I14</f>
@@ -6966,11 +6968,11 @@
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="0"/>
-        <v>3.7109375E-2</v>
+        <v>8.0078125E-2</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -6998,7 +7000,7 @@
       </c>
       <c r="H15" s="14">
         <f>Warren!H15+Sean!H15+Rhett!H15+Jalpa!H15+Nataliya!H15+John!H15+Renee!H15+Dong!H15+Lee!H15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I15" s="14">
         <f>Warren!I15+Sean!I15+Rhett!I15+Jalpa!I15+Nataliya!I15+John!I15+Renee!I15+Dong!I15+Lee!I15</f>
@@ -7042,11 +7044,11 @@
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="0"/>
-        <v>4.6875E-2</v>
+        <v>7.03125E-2</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -7074,7 +7076,7 @@
       </c>
       <c r="H16" s="14">
         <f>Warren!H16+Sean!H16+Rhett!H16+Jalpa!H16+Nataliya!H16+John!H16+Renee!H16+Dong!H16+Lee!H16</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I16" s="14">
         <f>Warren!I16+Sean!I16+Rhett!I16+Jalpa!I16+Nataliya!I16+John!I16+Renee!I16+Dong!I16+Lee!I16</f>
@@ -7118,11 +7120,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="0"/>
-        <v>4.9107142857142856E-2</v>
+        <v>0.12053571428571429</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -7150,7 +7152,7 @@
       </c>
       <c r="H17" s="14">
         <f>Warren!H17+Sean!H17+Rhett!H17+Jalpa!H17+Nataliya!H17+John!H17+Renee!H17+Dong!H17+Lee!H17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="14">
         <f>Warren!I17+Sean!I17+Rhett!I17+Jalpa!I17+Nataliya!I17+John!I17+Renee!I17+Dong!I17+Lee!I17</f>
@@ -7194,11 +7196,11 @@
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="0"/>
-        <v>7.8125E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="10" customFormat="1">
@@ -7219,7 +7221,7 @@
       </c>
       <c r="H18" s="13">
         <f t="shared" ref="H18:R18" si="2">SUM(H6:H17)</f>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="I18" s="13">
         <f t="shared" si="2"/>
@@ -7264,11 +7266,11 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13">
         <f t="shared" si="1"/>
-        <v>765</v>
+        <v>1530</v>
       </c>
       <c r="U18" s="12">
         <f t="shared" si="0"/>
-        <v>6.8696120689655166E-2</v>
+        <v>0.13739224137931033</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1">
@@ -7290,7 +7292,7 @@
       </c>
       <c r="H19" s="26">
         <f xml:space="preserve"> IF(H18=0, 0,(H18-E19)/H18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="I19" s="26">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-E19)/I18)</f>
@@ -7492,7 +7494,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="6">
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A1:B1"/>
@@ -7516,7 +7517,6 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7913,7 +7913,6 @@
       <c r="H52" s="61"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="A1:H1"/>
@@ -7932,11 +7931,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -8136,7 +8134,9 @@
       <c r="G6" s="14">
         <v>16</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="14">
+        <v>16</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -8510,7 +8510,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="0"/>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -8705,7 +8705,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -8761,7 +8761,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -8805,7 +8805,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -8824,11 +8823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9007,7 +9005,9 @@
       <c r="G6" s="3">
         <v>50</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3">
+        <v>50</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -9020,11 +9020,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="6">
         <f>SUM(G6:R6)</f>
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="U6" s="26">
         <f t="shared" ref="U6:U12" si="0">T6/MAX(C6,1)</f>
-        <v>0.10416666666666667</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -9047,7 +9047,9 @@
       <c r="G7" s="3">
         <v>15</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -9060,11 +9062,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="U7" s="26">
         <f t="shared" si="0"/>
-        <v>9.375E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -9315,7 +9317,9 @@
       <c r="G14" s="3">
         <v>10</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <v>10</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -9328,11 +9332,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="6">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="2"/>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -9393,7 +9397,9 @@
       <c r="G16" s="3">
         <v>5</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3">
+        <v>10</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -9406,11 +9412,11 @@
       <c r="R16" s="3"/>
       <c r="T16" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="2"/>
-        <v>3.125E-2</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -9472,7 +9478,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="3"/>
@@ -9516,11 +9522,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -9592,7 +9598,7 @@
       </c>
       <c r="H21" s="34">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I21" s="34">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -9642,7 +9648,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -9692,7 +9698,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -9736,7 +9742,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -9755,11 +9760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10084,7 +10088,9 @@
         <v>40344</v>
       </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>128</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -10097,11 +10103,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -10394,7 +10400,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="3"/>
@@ -10438,11 +10444,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -10662,7 +10668,6 @@
       <c r="C24" s="26"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -10681,11 +10686,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10895,7 +10899,9 @@
       <c r="G7" s="3">
         <v>4</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -10908,11 +10914,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -11126,7 +11132,9 @@
       <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>4</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -11139,11 +11147,11 @@
       <c r="R13" s="3"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -11319,7 +11327,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -11363,11 +11371,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -11439,7 +11447,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -11489,7 +11497,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -11539,7 +11547,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -11583,7 +11591,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -11602,11 +11609,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11931,7 +11937,9 @@
         <v>40344</v>
       </c>
       <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>80</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -11944,11 +11952,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -12007,7 +12015,9 @@
         <v>40344</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="H12" s="14">
+        <v>80</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
@@ -12020,11 +12030,11 @@
       <c r="R12" s="14"/>
       <c r="T12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U12" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -12238,7 +12248,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -12282,11 +12292,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -12361,7 +12371,7 @@
       </c>
       <c r="H21" s="34">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I21" s="34">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -12411,7 +12421,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -12461,7 +12471,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -12505,7 +12515,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -12524,11 +12533,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12738,7 +12746,9 @@
       <c r="G7" s="14">
         <v>20</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="14">
+        <v>20</v>
+      </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
@@ -12751,11 +12761,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -12969,7 +12979,9 @@
       <c r="G13" s="14">
         <v>17</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="14">
+        <v>20</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -12982,11 +12994,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>8.5000000000000006E-2</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -13164,7 +13176,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -13208,11 +13220,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>7.7083333333333337E-2</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -13287,7 +13299,7 @@
       </c>
       <c r="H21" s="34">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="I21" s="34">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -13337,7 +13349,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>403</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -13387,7 +13399,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -13431,7 +13443,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -13453,11 +13464,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13972,7 +13982,9 @@
       <c r="G15" s="14">
         <v>16</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="14">
+        <v>16</v>
+      </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
@@ -13985,11 +13997,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.10526315789473684</v>
+        <v>0.21052631578947367</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -14050,7 +14062,9 @@
       <c r="G17" s="14">
         <v>16</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14">
+        <v>16</v>
+      </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
@@ -14063,11 +14077,11 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
@@ -14214,7 +14228,7 @@
       </c>
       <c r="H21" s="34">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>38.4</v>
       </c>
       <c r="I21" s="34">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -14264,7 +14278,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -14314,7 +14328,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -14358,7 +14372,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -14377,12 +14390,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="17140" topLeftCell="V1"/>
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I8" sqref="I8"/>
       <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -14632,7 +14644,9 @@
       <c r="G8" s="14">
         <v>160</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="14">
+        <v>80</v>
+      </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
@@ -14645,11 +14659,11 @@
       <c r="R8" s="14"/>
       <c r="T8" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="U8" s="26">
         <f t="shared" ref="U8:U18" si="1">T8/MAX(C8,1)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -14822,7 +14836,9 @@
         <v>40344</v>
       </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="14">
+        <v>80</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -14835,11 +14851,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -15015,7 +15031,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -15059,11 +15075,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -15141,7 +15157,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -15194,7 +15210,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -15247,7 +15263,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -15291,7 +15307,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
@@ -15310,11 +15325,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15641,7 +15655,9 @@
       <c r="G10" s="14">
         <v>0</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="14">
+        <v>160</v>
+      </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -15654,11 +15670,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -15948,7 +15964,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
@@ -15992,11 +16008,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -16071,7 +16087,7 @@
       </c>
       <c r="H21" s="6">
         <f>IF(H23 = 0, 0, (C18-SUM(G18:H18))/(MONTH(N1-H5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="I21" s="6">
         <f ca="1">IF(I23 = 0, 0, (C18-SUM(G18:I18))/(MONTH(N1-I5)))</f>
@@ -16121,7 +16137,7 @@
       </c>
       <c r="H22" s="6">
         <f>IF(H23=0, 0,C18-SUM(G18:H18))</f>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="I22" s="6">
         <f ca="1">IF(I23=0, 0,C18-SUM(G18:I18))</f>
@@ -16171,7 +16187,7 @@
       </c>
       <c r="H23" s="6">
         <f>'Project Summary'!H16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="I23" s="6">
         <f ca="1">'Project Summary'!I16</f>
@@ -16215,7 +16231,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>

</xml_diff>

<commit_message>
added resource hours for October
</commit_message>
<xml_diff>
--- a/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
+++ b/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12720" yWindow="6100" windowWidth="28980" windowHeight="18860" tabRatio="921" activeTab="15"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16280" tabRatio="921"/>
   </bookViews>
   <sheets>
     <sheet name="Warren" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,11 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
   <si>
-    <t>Manager</t>
+    <t>Kruttik Aggarwal and Gaurav Gupta</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Kruttik Aggarwal</t>
+    <t>Manager</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
@@ -374,8 +374,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1131,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1313,8 +1316,12 @@
       <c r="H6" s="3">
         <v>12</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3">
+        <v>12</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1325,11 +1332,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="40">
         <f>SUM(G6:R6)</f>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="U6" s="4">
         <f>T6/MAX(C6,1)</f>
-        <v>0.14583333333333334</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -1356,8 +1363,12 @@
       <c r="H7" s="3">
         <v>8</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>8</v>
+      </c>
+      <c r="J7" s="3">
+        <v>8</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1368,11 +1379,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="40">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="U7" s="4">
         <f>T7/MAX(C7,1)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1628,8 +1639,12 @@
       <c r="H14" s="3">
         <v>8</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>8</v>
+      </c>
+      <c r="J14" s="3">
+        <v>8</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1640,11 +1655,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="40">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1786,11 +1801,11 @@
       </c>
       <c r="I18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K18" s="79">
         <f t="shared" si="2"/>
@@ -1826,11 +1841,11 @@
       </c>
       <c r="T18" s="40">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -1851,11 +1866,11 @@
       </c>
       <c r="I19" s="4">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="J19" s="4">
         <f xml:space="preserve"> IF(J18=0, 0,(J18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="K19" s="4">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-F18)/F18)</f>
@@ -2071,7 +2086,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2285,7 +2300,9 @@
       <c r="H7" s="14">
         <v>8</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="14">
+        <v>8</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
@@ -2297,11 +2314,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2707,7 +2724,7 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
@@ -2747,11 +2764,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="28" hidden="1">
@@ -2978,6 +2995,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2991,7 +3009,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3204,8 +3222,12 @@
       <c r="H7" s="14">
         <v>12</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="I7" s="14">
+        <v>12</v>
+      </c>
+      <c r="J7" s="14">
+        <v>12</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
@@ -3216,11 +3238,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.1796875</v>
+        <v>0.3671875</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3476,8 +3498,12 @@
       <c r="H14" s="14">
         <v>4</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="I14" s="14">
+        <v>4</v>
+      </c>
+      <c r="J14" s="14">
+        <v>4</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
@@ -3488,11 +3514,11 @@
       <c r="R14" s="14"/>
       <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="1"/>
-        <v>0.140625</v>
+        <v>0.265625</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3518,8 +3544,12 @@
       <c r="H15" s="14">
         <v>6</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="I15" s="14">
+        <v>6</v>
+      </c>
+      <c r="J15" s="14">
+        <v>6</v>
+      </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
@@ -3530,11 +3560,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3560,8 +3590,12 @@
       <c r="H16" s="14">
         <v>6</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="I16" s="14">
+        <v>6</v>
+      </c>
+      <c r="J16" s="14">
+        <v>6</v>
+      </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
@@ -3572,11 +3606,11 @@
       <c r="R16" s="14"/>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="1"/>
-        <v>0.1875</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3602,8 +3636,12 @@
       <c r="H17" s="14">
         <v>5</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="I17" s="14">
+        <v>5</v>
+      </c>
+      <c r="J17" s="14">
+        <v>5</v>
+      </c>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
@@ -3614,11 +3652,11 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.15625</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
@@ -3646,11 +3684,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -3686,11 +3724,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -3711,11 +3749,11 @@
       </c>
       <c r="I19" s="26">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="J19" s="26">
         <f xml:space="preserve"> IF(J18=0, 0,(J18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K19" s="26">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-F18)/F18)</f>
@@ -3914,6 +3952,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="C18" formulaRange="1"/>
   </ignoredErrors>
@@ -3930,7 +3969,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3987,7 +4026,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
@@ -4296,8 +4335,12 @@
       <c r="H11" s="14">
         <v>160</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="I11" s="14">
+        <v>160</v>
+      </c>
+      <c r="J11" s="14">
+        <v>80</v>
+      </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
@@ -4308,11 +4351,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>400</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -4373,7 +4416,9 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="14">
+        <v>80</v>
+      </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -4384,11 +4429,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -4568,11 +4613,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -4608,11 +4653,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>580</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.13541666666666666</v>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -5025,11 +5070,11 @@
       </c>
       <c r="I4" s="43">
         <f>Warren!I18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J4" s="43">
         <f>Warren!J18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K4" s="43">
         <f>Warren!K18</f>
@@ -5065,11 +5110,11 @@
       </c>
       <c r="S4" s="88">
         <f t="shared" ref="S4:S15" si="0">SUM(G4:R4)</f>
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="T4" s="28">
         <f>S4/MAX(1,D4)</f>
-        <v>0.14583333333333334</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5106,11 +5151,11 @@
       </c>
       <c r="I5" s="43">
         <f>Sean!I18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J5" s="43">
         <f>Sean!J18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K5" s="43">
         <f>Sean!K18</f>
@@ -5146,11 +5191,11 @@
       </c>
       <c r="S5" s="88">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ref="T5:T16" si="1">S5/MAX(1,D5)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5187,11 +5232,11 @@
       </c>
       <c r="I6" s="43">
         <f>Rhett!I18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="J6" s="43">
         <f>Rhett!J18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="K6" s="43">
         <f>Rhett!K18</f>
@@ -5227,11 +5272,11 @@
       </c>
       <c r="S6" s="88">
         <f t="shared" si="0"/>
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5349,11 +5394,11 @@
       </c>
       <c r="I8" s="43">
         <f>Nataliya!I18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J8" s="43">
         <f>Nataliya!J18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K8" s="43">
         <f>Nataliya!K18</f>
@@ -5389,11 +5434,11 @@
       </c>
       <c r="S8" s="88">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5430,7 +5475,7 @@
       </c>
       <c r="I9" s="43">
         <f>John!I18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J9" s="43">
         <f ca="1">John!J23</f>
@@ -5511,11 +5556,11 @@
       </c>
       <c r="I10" s="43">
         <f>David!I18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J10" s="43">
         <f>David!J18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K10" s="43">
         <f>David!K18</f>
@@ -5551,11 +5596,11 @@
       </c>
       <c r="S10" s="88">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>0.16041666666666668</v>
+        <v>0.32708333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="40" customFormat="1">
@@ -5673,7 +5718,7 @@
       </c>
       <c r="I12" s="43">
         <f>Renee!I18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J12" s="43">
         <f>Renee!J18</f>
@@ -5713,11 +5758,11 @@
       </c>
       <c r="S12" s="88">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5754,11 +5799,11 @@
       </c>
       <c r="I13" s="43">
         <f>Dong!I18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J13" s="43">
         <f>Dong!J18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K13" s="43">
         <f>Dong!K18</f>
@@ -5794,11 +5839,11 @@
       </c>
       <c r="S13" s="88">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5835,11 +5880,11 @@
       </c>
       <c r="I14" s="43">
         <f>Lee!I18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J14" s="43">
         <f>Lee!J18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K14" s="43">
         <f>Lee!K18</f>
@@ -5875,11 +5920,11 @@
       </c>
       <c r="S14" s="88">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -5888,7 +5933,7 @@
       </c>
       <c r="B15" s="30" t="str">
         <f>'SB-Dev'!C2</f>
-        <v>Kruttik Aggarwal</v>
+        <v>Kruttik Aggarwal and Gaurav Gupta</v>
       </c>
       <c r="C15" s="40" t="str">
         <f>'SB-Dev'!C3</f>
@@ -5916,11 +5961,11 @@
       </c>
       <c r="I15" s="84">
         <f>'SB-Dev'!I18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J15" s="84">
         <f>'SB-Dev'!J18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K15" s="84">
         <f>'SB-Dev'!K18</f>
@@ -5956,11 +6001,11 @@
       </c>
       <c r="S15" s="88">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>580</v>
       </c>
       <c r="T15" s="28">
         <f t="shared" si="1"/>
-        <v>0.13541666666666666</v>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1">
@@ -6314,11 +6359,11 @@
       </c>
       <c r="I6" s="14">
         <f>Warren!I6+Sean!I6+Rhett!I6+Jalpa!I6+Nataliya!I6+John!I6+Renee!I6+Dong!I6+Lee!I6</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="J6" s="14">
         <f>Warren!J6+Sean!J6+Rhett!J6+Jalpa!J6+Nataliya!J6+John!J6+Renee!J6+Dong!J6+Lee!J6</f>
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="K6" s="14">
         <f>Warren!K6+Sean!K6+Rhett!K6+Jalpa!K6+Nataliya!K6+John!K6+Renee!K6+Dong!K6+Lee!K6</f>
@@ -6354,11 +6399,11 @@
       </c>
       <c r="T6">
         <f>SUM(G6:R6)</f>
-        <v>128</v>
+        <v>252</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" ref="U6:U18" si="0">T6/MAX(1,D6)</f>
-        <v>0.19047619047619047</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6391,11 +6436,11 @@
       </c>
       <c r="I7" s="14">
         <f>Warren!I7+Sean!I7+Rhett!I7+Jalpa!I7+Nataliya!I7+John!I7+Renee!I7+Dong!I7+Lee!I7</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J7" s="14">
         <f>Warren!J7+Sean!J7+Rhett!J7+Jalpa!J7+Nataliya!J7+John!J7+Renee!J7+Dong!J7+Lee!J7</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="K7" s="14">
         <f>Warren!K7+Sean!K7+Rhett!K7+Jalpa!K7+Nataliya!K7+John!K7+Renee!K7+Dong!K7+Lee!K7</f>
@@ -6431,11 +6476,11 @@
       </c>
       <c r="T7">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>120</v>
+        <v>196</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>0.13157894736842105</v>
+        <v>0.21491228070175439</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6622,11 +6667,11 @@
       </c>
       <c r="I10" s="14">
         <f>Warren!I10+Sean!I10+Rhett!I10+Jalpa!I10+Nataliya!I10+John!I10+Renee!I10+Dong!I10+Lee!I10</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="J10" s="14">
         <f>Warren!J10+Sean!J10+Rhett!J10+Jalpa!J10+Nataliya!J10+John!J10+Renee!J10+Dong!J10+Lee!J10</f>
-        <v>0</v>
+        <v>288</v>
       </c>
       <c r="K10" s="14">
         <f>Warren!K10+Sean!K10+Rhett!K10+Jalpa!K10+Nataliya!K10+John!K10+Renee!K10+Dong!K10+Lee!K10</f>
@@ -6662,11 +6707,11 @@
       </c>
       <c r="T10">
         <f t="shared" si="1"/>
-        <v>368</v>
+        <v>1004</v>
       </c>
       <c r="U10" s="11">
         <f t="shared" si="0"/>
-        <v>368</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6699,11 +6744,11 @@
       </c>
       <c r="I11" s="14">
         <f>Warren!I11+Sean!I11+Rhett!I11+Jalpa!I11+Nataliya!I11+John!I11+Renee!I11+Dong!I11+Lee!I11</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J11" s="14">
         <f>Warren!J11+Sean!J11+Rhett!J11+Jalpa!J11+Nataliya!J11+John!J11+Renee!J11+Dong!J11+Lee!J11</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K11" s="14">
         <f>Warren!K11+Sean!K11+Rhett!K11+Jalpa!K11+Nataliya!K11+John!K11+Renee!K11+Dong!K11+Lee!K11</f>
@@ -6739,11 +6784,11 @@
       </c>
       <c r="T11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="U11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="28">
@@ -6776,7 +6821,7 @@
       </c>
       <c r="I12" s="14">
         <f>Warren!I12+Sean!I12+Rhett!I12+Jalpa!I12+Nataliya!I12+John!I12+Renee!I12+Dong!I12+Lee!I12</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J12" s="14">
         <f>Warren!J12+Sean!J12+Rhett!J12+Jalpa!J12+Nataliya!J12+John!J12+Renee!J12+Dong!J12+Lee!J12</f>
@@ -6816,11 +6861,11 @@
       </c>
       <c r="T12">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="U12" s="11">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6852,11 +6897,11 @@
       </c>
       <c r="I13" s="14">
         <f>Warren!I13+Sean!I13+Rhett!I13+Jalpa!I13+Nataliya!I13+John!I13+Renee!I13+Dong!I13+Lee!I13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="J13" s="14">
         <f>Warren!J13+Sean!J13+Rhett!J13+Jalpa!J13+Nataliya!J13+John!J13+Renee!J13+Dong!J13+Lee!J13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="K13" s="14">
         <f>Warren!K13+Sean!K13+Rhett!K13+Jalpa!K13+Nataliya!K13+John!K13+Renee!K13+Dong!K13+Lee!K13</f>
@@ -6892,11 +6937,11 @@
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>256</v>
       </c>
       <c r="U13" s="11">
         <f t="shared" si="0"/>
-        <v>1.8333333333333333</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28">
@@ -6928,11 +6973,11 @@
       </c>
       <c r="I14" s="14">
         <f>Warren!I14+Sean!I14+Rhett!I14+Jalpa!I14+Nataliya!I14+John!I14+Renee!I14+Dong!I14+Lee!I14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="J14" s="14">
         <f>Warren!J14+Sean!J14+Rhett!J14+Jalpa!J14+Nataliya!J14+John!J14+Renee!J14+Dong!J14+Lee!J14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K14" s="14">
         <f>Warren!K14+Sean!K14+Rhett!K14+Jalpa!K14+Nataliya!K14+John!K14+Renee!K14+Dong!K14+Lee!K14</f>
@@ -6968,11 +7013,11 @@
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="0"/>
-        <v>8.0078125E-2</v>
+        <v>0.205078125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -7004,11 +7049,11 @@
       </c>
       <c r="I15" s="14">
         <f>Warren!I15+Sean!I15+Rhett!I15+Jalpa!I15+Nataliya!I15+John!I15+Renee!I15+Dong!I15+Lee!I15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J15" s="14">
         <f>Warren!J15+Sean!J15+Rhett!J15+Jalpa!J15+Nataliya!J15+John!J15+Renee!J15+Dong!J15+Lee!J15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K15" s="14">
         <f>Warren!K15+Sean!K15+Rhett!K15+Jalpa!K15+Nataliya!K15+John!K15+Renee!K15+Dong!K15+Lee!K15</f>
@@ -7044,11 +7089,11 @@
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="0"/>
-        <v>7.03125E-2</v>
+        <v>0.1171875</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -7080,11 +7125,11 @@
       </c>
       <c r="I16" s="14">
         <f>Warren!I16+Sean!I16+Rhett!I16+Jalpa!I16+Nataliya!I16+John!I16+Renee!I16+Dong!I16+Lee!I16</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J16" s="14">
         <f>Warren!J16+Sean!J16+Rhett!J16+Jalpa!J16+Nataliya!J16+John!J16+Renee!J16+Dong!J16+Lee!J16</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K16" s="14">
         <f>Warren!K16+Sean!K16+Rhett!K16+Jalpa!K16+Nataliya!K16+John!K16+Renee!K16+Dong!K16+Lee!K16</f>
@@ -7120,11 +7165,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="0"/>
-        <v>0.12053571428571429</v>
+        <v>0.17410714285714285</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -7156,11 +7201,11 @@
       </c>
       <c r="I17" s="14">
         <f>Warren!I17+Sean!I17+Rhett!I17+Jalpa!I17+Nataliya!I17+John!I17+Renee!I17+Dong!I17+Lee!I17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J17" s="14">
         <f>Warren!J17+Sean!J17+Rhett!J17+Jalpa!J17+Nataliya!J17+John!J17+Renee!J17+Dong!J17+Lee!J17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K17" s="14">
         <f>Warren!K17+Sean!K17+Rhett!K17+Jalpa!K17+Nataliya!K17+John!K17+Renee!K17+Dong!K17+Lee!K17</f>
@@ -7196,11 +7241,11 @@
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="0"/>
-        <v>0.15625</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="10" customFormat="1">
@@ -7225,11 +7270,11 @@
       </c>
       <c r="I18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="J18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>597</v>
       </c>
       <c r="K18" s="13">
         <f t="shared" si="2"/>
@@ -7266,11 +7311,11 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13">
         <f t="shared" si="1"/>
-        <v>1530</v>
+        <v>2892</v>
       </c>
       <c r="U18" s="12">
         <f t="shared" si="0"/>
-        <v>0.13739224137931033</v>
+        <v>0.25969827586206895</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1">
@@ -7296,11 +7341,11 @@
       </c>
       <c r="I19" s="26">
         <f xml:space="preserve"> IF(I18=0, 0,(I18-E19)/I18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="J19" s="26">
         <f xml:space="preserve"> IF(J18=0, 0,(J18-E19)/J18)</f>
-        <v>0</v>
+        <v>-0.55443886097152428</v>
       </c>
       <c r="K19" s="26">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-E19)/K18)</f>
@@ -7933,8 +7978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -8009,7 +8054,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="91"/>
       <c r="E3" s="91"/>
@@ -8137,8 +8182,12 @@
       <c r="H6" s="14">
         <v>16</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="14">
+        <v>16</v>
+      </c>
+      <c r="J6" s="14">
+        <v>16</v>
+      </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
@@ -8514,11 +8563,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="0"/>
@@ -8826,7 +8875,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9008,8 +9057,12 @@
       <c r="H6" s="3">
         <v>50</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3">
+        <v>50</v>
+      </c>
+      <c r="J6" s="3">
+        <v>50</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -9020,11 +9073,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="6">
         <f>SUM(G6:R6)</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="U6" s="26">
         <f t="shared" ref="U6:U12" si="0">T6/MAX(C6,1)</f>
-        <v>0.20833333333333334</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -9050,8 +9103,12 @@
       <c r="H7" s="3">
         <v>10</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3">
+        <v>10</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -9062,11 +9119,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="U7" s="26">
         <f t="shared" si="0"/>
-        <v>0.15625</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -9320,8 +9377,12 @@
       <c r="H14" s="3">
         <v>10</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3">
+        <v>20</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -9332,11 +9393,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="6">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="2"/>
-        <v>0.125</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -9482,11 +9543,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="3"/>
@@ -9522,11 +9583,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -9763,7 +9824,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10091,8 +10152,12 @@
       <c r="H10" s="14">
         <v>128</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="14">
+        <v>128</v>
+      </c>
+      <c r="J10" s="14">
+        <v>128</v>
+      </c>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
@@ -10103,11 +10168,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>384</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="0"/>
-        <v>128</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -10404,11 +10469,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="3"/>
@@ -10444,11 +10509,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -10689,7 +10754,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10902,8 +10967,12 @@
       <c r="H7" s="3">
         <v>4</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="3">
+        <v>4</v>
+      </c>
+      <c r="J7" s="3">
+        <v>4</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -10914,11 +10983,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -11135,8 +11204,12 @@
       <c r="H13" s="3">
         <v>4</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3">
+        <v>4</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -11147,11 +11220,11 @@
       <c r="R13" s="3"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -11331,11 +11404,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -11371,11 +11444,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -11612,7 +11685,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11940,7 +12013,9 @@
       <c r="H10" s="14">
         <v>80</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14">
+        <v>60</v>
+      </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -11952,11 +12027,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -11978,7 +12053,9 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="14">
+        <v>100</v>
+      </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -11990,11 +12067,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -12252,7 +12329,7 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
@@ -12292,11 +12369,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>480</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -12536,7 +12613,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12749,8 +12826,12 @@
       <c r="H7" s="14">
         <v>20</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="I7" s="14">
+        <v>20</v>
+      </c>
+      <c r="J7" s="14">
+        <v>20</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
@@ -12761,11 +12842,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -12982,8 +13063,12 @@
       <c r="H13" s="14">
         <v>20</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="I13" s="14">
+        <v>20</v>
+      </c>
+      <c r="J13" s="14">
+        <v>20</v>
+      </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -12994,11 +13079,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.185</v>
+        <v>0.38500000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -13180,11 +13265,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -13220,11 +13305,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16041666666666668</v>
+        <v>0.32708333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -13467,7 +13552,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13985,7 +14070,9 @@
       <c r="H15" s="14">
         <v>16</v>
       </c>
-      <c r="I15" s="14"/>
+      <c r="I15" s="14">
+        <v>16</v>
+      </c>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
@@ -13997,11 +14084,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.21052631578947367</v>
+        <v>0.31578947368421051</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -14065,7 +14152,9 @@
       <c r="H17" s="14">
         <v>16</v>
       </c>
-      <c r="I17" s="14"/>
+      <c r="I17" s="14">
+        <v>16</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -14077,11 +14166,11 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
@@ -14393,8 +14482,8 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="17140" topLeftCell="V1"/>
-      <selection activeCell="I8" sqref="I8"/>
+      <pane xSplit="20120" topLeftCell="V1"/>
+      <selection activeCell="J12" sqref="J12"/>
       <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -14762,7 +14851,9 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="14">
+        <v>80</v>
+      </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
@@ -14773,11 +14864,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -14799,7 +14890,9 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="14">
+        <v>80</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
@@ -14811,11 +14904,11 @@
       <c r="R12" s="14"/>
       <c r="T12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="U12" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -14839,8 +14932,12 @@
       <c r="H13" s="14">
         <v>80</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="I13" s="14">
+        <v>80</v>
+      </c>
+      <c r="J13" s="14">
+        <v>80</v>
+      </c>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -14851,11 +14948,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -15035,11 +15132,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -15075,11 +15172,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -15328,7 +15425,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15658,8 +15755,12 @@
       <c r="H10" s="14">
         <v>160</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="14">
+        <v>160</v>
+      </c>
+      <c r="J10" s="14">
+        <v>160</v>
+      </c>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
@@ -15670,11 +15771,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>480</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -15968,11 +16069,11 @@
       </c>
       <c r="I18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
@@ -16008,11 +16109,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>640</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -16239,6 +16340,7 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
status updates for November
</commit_message>
<xml_diff>
--- a/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
+++ b/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16280" tabRatio="921"/>
+    <workbookView xWindow="20700" yWindow="4200" windowWidth="24800" windowHeight="16280" tabRatio="921" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Warren" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,10 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
+  <si>
+    <t>Ram Chilukuri</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
   <si>
     <t>Kruttik Aggarwal and Gaurav Gupta</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -365,20 +369,13 @@
     <t>System Admin</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
-  <si>
-    <t>Ram Chilukuri</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1134,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1157,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -1170,35 +1167,35 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
         <v>40344</v>
       </c>
       <c r="Q1" s="94" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R1" s="94"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -1208,32 +1205,32 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -1322,7 +1319,9 @@
       <c r="J6" s="3">
         <v>12</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <v>20</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -1332,11 +1331,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="40">
         <f>SUM(G6:R6)</f>
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="U6" s="4">
         <f>T6/MAX(C6,1)</f>
-        <v>0.27083333333333331</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -1645,7 +1644,9 @@
       <c r="J14" s="3">
         <v>8</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="3">
+        <v>8</v>
+      </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1655,11 +1656,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="40">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1778,7 +1779,7 @@
     </row>
     <row r="18" spans="1:21" hidden="1">
       <c r="A18" s="79" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="79"/>
       <c r="C18" s="79">
@@ -1809,7 +1810,7 @@
       </c>
       <c r="K18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="L18" s="79">
         <f t="shared" si="2"/>
@@ -1841,16 +1842,16 @@
       </c>
       <c r="T18" s="40">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>0.36458333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -1874,7 +1875,7 @@
       </c>
       <c r="K19" s="4">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="L19" s="4">
         <f xml:space="preserve"> IF(L18=0, 0,(L18-F18)/F18)</f>
@@ -1907,7 +1908,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="40">
         <v>192</v>
@@ -1932,7 +1933,7 @@
       </c>
       <c r="K21" s="80">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>34.857142857142854</v>
       </c>
       <c r="L21" s="80">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -1982,7 +1983,7 @@
       </c>
       <c r="K22" s="40">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="L22" s="40">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -2032,7 +2033,7 @@
       </c>
       <c r="K23" s="40">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="40">
         <f>'Project Summary'!L16</f>
@@ -2086,7 +2087,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2111,7 +2112,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -2124,14 +2125,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -2140,15 +2141,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -2157,29 +2158,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -2303,8 +2304,12 @@
       <c r="I7" s="14">
         <v>8</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="14">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14">
+        <v>8</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -2314,11 +2319,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2701,7 +2706,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -2728,11 +2733,11 @@
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -2764,16 +2769,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="28" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -2830,7 +2835,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -2855,7 +2860,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -2905,7 +2910,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -2955,7 +2960,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -2995,7 +3000,6 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3009,7 +3013,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3034,7 +3038,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -3047,14 +3051,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -3063,15 +3067,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -3080,29 +3084,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -3228,7 +3232,9 @@
       <c r="J7" s="14">
         <v>12</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>12</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -3238,11 +3244,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.3671875</v>
+        <v>0.4609375</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3504,7 +3510,9 @@
       <c r="J14" s="14">
         <v>4</v>
       </c>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14">
+        <v>4</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
@@ -3514,11 +3522,11 @@
       <c r="R14" s="14"/>
       <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="1"/>
-        <v>0.265625</v>
+        <v>0.328125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3550,7 +3558,9 @@
       <c r="J15" s="14">
         <v>6</v>
       </c>
-      <c r="K15" s="14"/>
+      <c r="K15" s="14">
+        <v>6</v>
+      </c>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
@@ -3560,11 +3570,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3596,7 +3606,9 @@
       <c r="J16" s="14">
         <v>6</v>
       </c>
-      <c r="K16" s="14"/>
+      <c r="K16" s="14">
+        <v>6</v>
+      </c>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
@@ -3606,11 +3618,11 @@
       <c r="R16" s="14"/>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3642,7 +3654,9 @@
       <c r="J17" s="14">
         <v>5</v>
       </c>
-      <c r="K17" s="14"/>
+      <c r="K17" s="14">
+        <v>5</v>
+      </c>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -3652,16 +3666,16 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.3125</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -3692,7 +3706,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -3724,16 +3738,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -3757,7 +3771,7 @@
       </c>
       <c r="K19" s="26">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="L19" s="26">
         <f xml:space="preserve"> IF(L18=0, 0,(L18-F18)/F18)</f>
@@ -3790,7 +3804,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -3812,7 +3826,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>43.428571428571431</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -3862,7 +3876,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -3912,7 +3926,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -3952,7 +3966,6 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="C18" formulaRange="1"/>
   </ignoredErrors>
@@ -3969,7 +3982,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3994,7 +4007,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -4007,14 +4020,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -4023,15 +4036,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -4041,29 +4054,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -4341,7 +4354,9 @@
       <c r="J11" s="14">
         <v>80</v>
       </c>
-      <c r="K11" s="14"/>
+      <c r="K11" s="14">
+        <v>80</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -4351,11 +4366,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>480</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -4419,7 +4434,9 @@
       <c r="J13" s="14">
         <v>80</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="14">
+        <v>80</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -4429,11 +4446,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -4590,7 +4607,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -4621,7 +4638,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -4653,16 +4670,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>740</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.30208333333333331</v>
+        <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -4719,7 +4736,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1">
       <c r="B20" s="40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -4741,7 +4758,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>168.57142857142858</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -4791,7 +4808,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -4841,7 +4858,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -4910,11 +4927,11 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="96" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D1" s="96"/>
       <c r="E1" s="96"/>
@@ -4922,13 +4939,13 @@
       <c r="G1" s="96"/>
       <c r="H1" s="96"/>
       <c r="K1" s="30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="42">
         <v>39980</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="42">
         <v>40344</v>
@@ -4936,102 +4953,102 @@
     </row>
     <row r="2" spans="1:20" s="38" customFormat="1">
       <c r="G2" s="38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P2" s="38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T2" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="15" customFormat="1">
       <c r="A3" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>75</v>
-      </c>
       <c r="K3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
@@ -5078,7 +5095,7 @@
       </c>
       <c r="K4" s="43">
         <f>Warren!K18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="L4" s="43">
         <f>Warren!L18</f>
@@ -5110,11 +5127,11 @@
       </c>
       <c r="S4" s="88">
         <f t="shared" ref="S4:S15" si="0">SUM(G4:R4)</f>
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="T4" s="28">
         <f>S4/MAX(1,D4)</f>
-        <v>0.29166666666666669</v>
+        <v>0.36458333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5159,7 +5176,7 @@
       </c>
       <c r="K5" s="43">
         <f>Sean!K18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L5" s="43">
         <f>Sean!L18</f>
@@ -5191,11 +5208,11 @@
       </c>
       <c r="S5" s="88">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ref="T5:T16" si="1">S5/MAX(1,D5)</f>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5240,7 +5257,7 @@
       </c>
       <c r="K6" s="43">
         <f>Rhett!K18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="L6" s="43">
         <f>Rhett!L18</f>
@@ -5272,11 +5289,11 @@
       </c>
       <c r="S6" s="88">
         <f t="shared" si="0"/>
-        <v>512</v>
+        <v>640</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5317,11 +5334,11 @@
       </c>
       <c r="J7" s="43">
         <f>Jalpa!J18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K7" s="43">
         <f>Jalpa!K18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L7" s="43">
         <f>Jalpa!L18</f>
@@ -5402,7 +5419,7 @@
       </c>
       <c r="K8" s="43">
         <f>Nataliya!K18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L8" s="43">
         <f>Nataliya!L18</f>
@@ -5434,11 +5451,11 @@
       </c>
       <c r="S8" s="88">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5483,7 +5500,7 @@
       </c>
       <c r="K9" s="43">
         <f>John!K18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L9" s="43">
         <f>John!L18</f>
@@ -5564,7 +5581,7 @@
       </c>
       <c r="K10" s="43">
         <f>David!K18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L10" s="43">
         <f>David!L18</f>
@@ -5596,11 +5613,11 @@
       </c>
       <c r="S10" s="88">
         <f t="shared" si="0"/>
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>0.32708333333333334</v>
+        <v>0.41041666666666665</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="40" customFormat="1">
@@ -5722,11 +5739,11 @@
       </c>
       <c r="J12" s="43">
         <f>Renee!J18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K12" s="43">
         <f>Renee!K18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L12" s="43">
         <f>Renee!L18</f>
@@ -5758,11 +5775,11 @@
       </c>
       <c r="S12" s="88">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5807,7 +5824,7 @@
       </c>
       <c r="K13" s="43">
         <f>Dong!K18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L13" s="43">
         <f>Dong!L18</f>
@@ -5839,11 +5856,11 @@
       </c>
       <c r="S13" s="88">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.20833333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5888,7 +5905,7 @@
       </c>
       <c r="K14" s="43">
         <f>Lee!K18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L14" s="43">
         <f>Lee!L18</f>
@@ -5920,14 +5937,14 @@
       </c>
       <c r="S14" s="88">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="28">
       <c r="A15" s="30">
         <v>12</v>
       </c>
@@ -5969,7 +5986,7 @@
       </c>
       <c r="K15" s="84">
         <f>'SB-Dev'!K18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L15" s="84">
         <f>'SB-Dev'!L18</f>
@@ -6001,16 +6018,16 @@
       </c>
       <c r="S15" s="88">
         <f t="shared" si="0"/>
-        <v>580</v>
+        <v>740</v>
       </c>
       <c r="T15" s="28">
         <f t="shared" si="1"/>
-        <v>0.30208333333333331</v>
+        <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1">
       <c r="A16" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -6038,7 +6055,7 @@
       </c>
       <c r="K16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L16" s="19">
         <f t="shared" si="2"/>
@@ -6079,7 +6096,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G22" s="30">
         <v>1</v>
@@ -6120,33 +6137,33 @@
     </row>
     <row r="24" spans="1:18" s="76" customFormat="1">
       <c r="A24" s="97" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="98"/>
       <c r="D24" s="76" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E24" s="76" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" s="76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6191,7 +6208,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="45" customFormat="1" ht="14.5" customHeight="1">
       <c r="A1" s="100" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="99" t="str">
@@ -6204,14 +6221,14 @@
       <c r="G1" s="85"/>
       <c r="H1" s="85"/>
       <c r="K1" s="47" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="86">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="86">
         <f>'Project Summary'!N1</f>
@@ -6230,103 +6247,103 @@
     </row>
     <row r="4" spans="1:21" s="35" customFormat="1">
       <c r="A4" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" s="35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="35" customFormat="1">
       <c r="A5" s="101"/>
       <c r="G5" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6335,7 +6352,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="83">
         <f>Warren!C6+Sean!C6+Rhett!C6+Jalpa!C6+Nataliya!C6+John!C6+Renee!C6+Dong!C6+Lee!C6+'SB-Dev'!C6</f>
@@ -6367,7 +6384,7 @@
       </c>
       <c r="K6" s="14">
         <f>Warren!K6+Sean!K6+Rhett!K6+Jalpa!K6+Nataliya!K6+John!K6+Renee!K6+Dong!K6+Lee!K6</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="L6" s="14">
         <f>Warren!L6+Sean!L6+Rhett!L6+Jalpa!L6+Nataliya!L6+John!L6+Renee!L6+Dong!L6+Lee!L6</f>
@@ -6399,11 +6416,11 @@
       </c>
       <c r="T6">
         <f>SUM(G6:R6)</f>
-        <v>252</v>
+        <v>322</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" ref="U6:U18" si="0">T6/MAX(1,D6)</f>
-        <v>0.375</v>
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6412,7 +6429,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="83">
         <f>Warren!C7+Sean!C7+Rhett!C7+Jalpa!C7+Nataliya!C7+John!C7+Renee!C7+Dong!C7+Lee!C7+'SB-Dev'!C7</f>
@@ -6440,11 +6457,11 @@
       </c>
       <c r="J7" s="14">
         <f>Warren!J7+Sean!J7+Rhett!J7+Jalpa!J7+Nataliya!J7+John!J7+Renee!J7+Dong!J7+Lee!J7</f>
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="K7" s="14">
         <f>Warren!K7+Sean!K7+Rhett!K7+Jalpa!K7+Nataliya!K7+John!K7+Renee!K7+Dong!K7+Lee!K7</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="L7" s="14">
         <f>Warren!L7+Sean!L7+Rhett!L7+Jalpa!L7+Nataliya!L7+John!L7+Renee!L7+Dong!L7+Lee!L7</f>
@@ -6476,11 +6493,11 @@
       </c>
       <c r="T7">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>0.21491228070175439</v>
+        <v>0.26096491228070173</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6489,7 +6506,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" s="83">
         <f>Warren!C8+Sean!C8+Rhett!C8+Jalpa!C8+Nataliya!C8+John!C8+Renee!C8+Dong!C8+Lee!C8+'SB-Dev'!C8</f>
@@ -6566,7 +6583,7 @@
         <v>3.1</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D9" s="83">
         <f>Warren!C9+Sean!C9+Rhett!C9+Jalpa!C9+Nataliya!C9+John!C9+Renee!C9+Dong!C9+Lee!C9+'SB-Dev'!C9</f>
@@ -6643,7 +6660,7 @@
         <v>3.2</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D10" s="83">
         <f>Warren!C10+Sean!C10+Rhett!C10+Jalpa!C10+Nataliya!C10+John!C10+Renee!C10+Dong!C10+Lee!C10+'SB-Dev'!C10</f>
@@ -6671,11 +6688,11 @@
       </c>
       <c r="J10" s="14">
         <f>Warren!J10+Sean!J10+Rhett!J10+Jalpa!J10+Nataliya!J10+John!J10+Renee!J10+Dong!J10+Lee!J10</f>
-        <v>288</v>
+        <v>328</v>
       </c>
       <c r="K10" s="14">
         <f>Warren!K10+Sean!K10+Rhett!K10+Jalpa!K10+Nataliya!K10+John!K10+Renee!K10+Dong!K10+Lee!K10</f>
-        <v>0</v>
+        <v>288</v>
       </c>
       <c r="L10" s="14">
         <f>Warren!L10+Sean!L10+Rhett!L10+Jalpa!L10+Nataliya!L10+John!L10+Renee!L10+Dong!L10+Lee!L10</f>
@@ -6707,11 +6724,11 @@
       </c>
       <c r="T10">
         <f t="shared" si="1"/>
-        <v>1004</v>
+        <v>1332</v>
       </c>
       <c r="U10" s="11">
         <f t="shared" si="0"/>
-        <v>1004</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6720,7 +6737,7 @@
         <v>3.3</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="83">
         <f>Warren!C11+Sean!C11+Rhett!C11+Jalpa!C11+Nataliya!C11+John!C11+Renee!C11+Dong!C11+Lee!C11+'SB-Dev'!C11</f>
@@ -6748,11 +6765,11 @@
       </c>
       <c r="J11" s="14">
         <f>Warren!J11+Sean!J11+Rhett!J11+Jalpa!J11+Nataliya!J11+John!J11+Renee!J11+Dong!J11+Lee!J11</f>
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="K11" s="14">
         <f>Warren!K11+Sean!K11+Rhett!K11+Jalpa!K11+Nataliya!K11+John!K11+Renee!K11+Dong!K11+Lee!K11</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="L11" s="14">
         <f>Warren!L11+Sean!L11+Rhett!L11+Jalpa!L11+Nataliya!L11+John!L11+Renee!L11+Dong!L11+Lee!L11</f>
@@ -6784,11 +6801,11 @@
       </c>
       <c r="T11">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>540</v>
       </c>
       <c r="U11" s="11">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="28">
@@ -6797,7 +6814,7 @@
         <v>3.4</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D12" s="83">
         <f>Warren!C12+Sean!C12+Rhett!C12+Jalpa!C12+Nataliya!C12+John!C12+Renee!C12+Dong!C12+Lee!C12+'SB-Dev'!C12</f>
@@ -6873,7 +6890,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="83">
         <f>Warren!C13+Sean!C13+Rhett!C13+Jalpa!C13+Nataliya!C13+John!C13+Renee!C13+Dong!C13+Lee!C13+'SB-Dev'!C13</f>
@@ -6905,7 +6922,7 @@
       </c>
       <c r="K13" s="14">
         <f>Warren!K13+Sean!K13+Rhett!K13+Jalpa!K13+Nataliya!K13+John!K13+Renee!K13+Dong!K13+Lee!K13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="L13" s="14">
         <f>Warren!L13+Sean!L13+Rhett!L13+Jalpa!L13+Nataliya!L13+John!L13+Renee!L13+Dong!L13+Lee!L13</f>
@@ -6937,11 +6954,11 @@
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>340</v>
       </c>
       <c r="U13" s="11">
         <f t="shared" si="0"/>
-        <v>5.333333333333333</v>
+        <v>7.083333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28">
@@ -6949,7 +6966,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D14" s="83">
         <f>Warren!C14+Sean!C14+Rhett!C14+Jalpa!C14+Nataliya!C14+John!C14+Renee!C14+Dong!C14+Lee!C14+'SB-Dev'!C14</f>
@@ -6981,7 +6998,7 @@
       </c>
       <c r="K14" s="14">
         <f>Warren!K14+Sean!K14+Rhett!K14+Jalpa!K14+Nataliya!K14+John!K14+Renee!K14+Dong!K14+Lee!K14</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L14" s="14">
         <f>Warren!L14+Sean!L14+Rhett!L14+Jalpa!L14+Nataliya!L14+John!L14+Renee!L14+Dong!L14+Lee!L14</f>
@@ -7013,11 +7030,11 @@
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="0"/>
-        <v>0.205078125</v>
+        <v>0.228515625</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -7025,7 +7042,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="83">
         <f>Warren!C15+Sean!C15+Rhett!C15+Jalpa!C15+Nataliya!C15+John!C15+Renee!C15+Dong!C15+Lee!C15+'SB-Dev'!C15</f>
@@ -7057,7 +7074,7 @@
       </c>
       <c r="K15" s="14">
         <f>Warren!K15+Sean!K15+Rhett!K15+Jalpa!K15+Nataliya!K15+John!K15+Renee!K15+Dong!K15+Lee!K15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L15" s="14">
         <f>Warren!L15+Sean!L15+Rhett!L15+Jalpa!L15+Nataliya!L15+John!L15+Renee!L15+Dong!L15+Lee!L15</f>
@@ -7089,11 +7106,11 @@
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="0"/>
-        <v>0.1171875</v>
+        <v>0.140625</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -7101,7 +7118,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" s="83">
         <f>Warren!C16+Sean!C16+Rhett!C16+Jalpa!C16+Nataliya!C16+John!C16+Renee!C16+Dong!C16+Lee!C16+'SB-Dev'!C16</f>
@@ -7133,7 +7150,7 @@
       </c>
       <c r="K16" s="14">
         <f>Warren!K16+Sean!K16+Rhett!K16+Jalpa!K16+Nataliya!K16+John!K16+Renee!K16+Dong!K16+Lee!K16</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L16" s="14">
         <f>Warren!L16+Sean!L16+Rhett!L16+Jalpa!L16+Nataliya!L16+John!L16+Renee!L16+Dong!L16+Lee!L16</f>
@@ -7165,11 +7182,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="0"/>
-        <v>0.17410714285714285</v>
+        <v>0.29017857142857145</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -7177,7 +7194,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="83">
         <f>Warren!C17+Sean!C17+Rhett!C17+Jalpa!C17+Nataliya!C17+John!C17+Renee!C17+Dong!C17+Lee!C17+'SB-Dev'!C17</f>
@@ -7209,7 +7226,7 @@
       </c>
       <c r="K17" s="14">
         <f>Warren!K17+Sean!K17+Rhett!K17+Jalpa!K17+Nataliya!K17+John!K17+Renee!K17+Dong!K17+Lee!K17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L17" s="14">
         <f>Warren!L17+Sean!L17+Rhett!L17+Jalpa!L17+Nataliya!L17+John!L17+Renee!L17+Dong!L17+Lee!L17</f>
@@ -7241,16 +7258,16 @@
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.390625</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="10" customFormat="1">
       <c r="A18" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -7274,11 +7291,11 @@
       </c>
       <c r="J18" s="13">
         <f t="shared" si="2"/>
-        <v>597</v>
+        <v>765</v>
       </c>
       <c r="K18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="L18" s="13">
         <f t="shared" si="2"/>
@@ -7311,16 +7328,16 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13">
         <f t="shared" si="1"/>
-        <v>2892</v>
+        <v>3825</v>
       </c>
       <c r="U18" s="12">
         <f t="shared" si="0"/>
-        <v>0.25969827586206895</v>
+        <v>0.34348060344827586</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="4">
@@ -7345,11 +7362,11 @@
       </c>
       <c r="J19" s="26">
         <f xml:space="preserve"> IF(J18=0, 0,(J18-E19)/J18)</f>
-        <v>-0.55443886097152428</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="K19" s="26">
         <f xml:space="preserve"> IF(K18=0, 0,(K18-E19)/K18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="L19" s="26">
         <f xml:space="preserve"> IF(L18=0, 0,(L18-E19)/L18)</f>
@@ -7382,7 +7399,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1">
       <c r="A21" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (D18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -7435,7 +7452,7 @@
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, D18-SUM(G18:G18))</f>
@@ -7488,7 +7505,7 @@
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1">
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -7978,15 +7995,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8001,14 +8018,14 @@
       <c r="I1" s="90"/>
       <c r="J1" s="90"/>
       <c r="K1" s="90" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8022,16 +8039,16 @@
     <row r="2" spans="1:18" ht="28">
       <c r="A2" s="90"/>
       <c r="B2" s="90" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="F2" s="90"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -8051,10 +8068,10 @@
     <row r="3" spans="1:18" ht="28">
       <c r="A3" s="90"/>
       <c r="B3" s="90" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="91"/>
       <c r="E3" s="91"/>
@@ -8094,19 +8111,19 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="92" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="92"/>
       <c r="G5" s="81" t="str">
@@ -8188,7 +8205,9 @@
       <c r="J6" s="14">
         <v>16</v>
       </c>
-      <c r="K6" s="14"/>
+      <c r="K6" s="14">
+        <v>16</v>
+      </c>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
@@ -8540,7 +8559,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -8571,7 +8590,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="0"/>
@@ -8604,7 +8623,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="90" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" s="90"/>
       <c r="C19" s="26">
@@ -8666,7 +8685,7 @@
     <row r="20" spans="1:18" ht="42">
       <c r="A20" s="6"/>
       <c r="B20" s="90" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -8710,7 +8729,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -8766,7 +8785,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -8822,7 +8841,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -8875,7 +8894,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8900,7 +8919,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8913,14 +8932,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8934,15 +8953,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -8952,10 +8971,10 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -8963,19 +8982,19 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -9063,7 +9082,9 @@
       <c r="J6" s="3">
         <v>50</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3">
+        <v>50</v>
+      </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -9073,11 +9094,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="6">
         <f>SUM(G6:R6)</f>
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="U6" s="26">
         <f t="shared" ref="U6:U12" si="0">T6/MAX(C6,1)</f>
-        <v>0.41666666666666669</v>
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -9109,7 +9130,9 @@
       <c r="J7" s="3">
         <v>10</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>10</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -9119,11 +9142,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="U7" s="26">
         <f t="shared" si="0"/>
-        <v>0.28125</v>
+        <v>0.34375</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -9463,7 +9486,9 @@
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3">
+        <v>20</v>
+      </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -9473,11 +9498,11 @@
       <c r="R16" s="3"/>
       <c r="T16" s="6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="2"/>
-        <v>9.375E-2</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -9520,7 +9545,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -9551,7 +9576,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="3"/>
@@ -9583,16 +9608,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>400</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -9649,7 +9674,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -9671,7 +9696,7 @@
       </c>
       <c r="K21" s="34">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L21" s="34">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -9721,7 +9746,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -9771,7 +9796,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -9824,7 +9849,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9849,7 +9874,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -9862,14 +9887,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
@@ -9878,15 +9903,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -9895,29 +9920,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="22" customFormat="1">
       <c r="A5" s="22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="81" t="str">
@@ -10158,7 +10183,9 @@
       <c r="J10" s="14">
         <v>128</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="14">
+        <v>128</v>
+      </c>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
@@ -10168,11 +10195,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="1"/>
-        <v>384</v>
+        <v>512</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="0"/>
-        <v>384</v>
+        <v>512</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -10446,7 +10473,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -10477,7 +10504,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="3"/>
@@ -10509,11 +10536,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>512</v>
+        <v>640</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -10572,7 +10599,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1">
         <v>960</v>
@@ -10754,7 +10781,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10779,7 +10806,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -10792,14 +10819,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -10808,15 +10835,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -10825,29 +10852,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -10973,7 +11000,9 @@
       <c r="J7" s="3">
         <v>4</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3">
+        <v>4</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -10983,11 +11012,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -11210,7 +11239,9 @@
       <c r="J13" s="3">
         <v>4</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3">
+        <v>4</v>
+      </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -11220,11 +11251,11 @@
       <c r="R13" s="3"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -11381,7 +11412,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -11412,7 +11443,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -11444,16 +11475,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -11510,7 +11541,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -11532,7 +11563,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -11582,7 +11613,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -11632,7 +11663,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -11685,7 +11716,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11710,7 +11741,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -11723,14 +11754,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -11739,15 +11770,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -11757,29 +11788,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12016,7 +12047,9 @@
       <c r="I10" s="14">
         <v>60</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="14">
+        <v>40</v>
+      </c>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
@@ -12027,11 +12060,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -12056,8 +12089,12 @@
       <c r="I11" s="14">
         <v>100</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="14">
+        <v>120</v>
+      </c>
+      <c r="K11" s="14">
+        <v>160</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -12067,11 +12104,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>380</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -12306,7 +12343,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -12333,11 +12370,11 @@
       </c>
       <c r="J18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -12369,16 +12406,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>800</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -12435,7 +12472,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -12460,7 +12497,7 @@
       </c>
       <c r="K21" s="34">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L21" s="34">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -12510,7 +12547,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -12560,7 +12597,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -12613,7 +12650,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12638,7 +12675,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -12651,14 +12688,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -12667,15 +12704,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -12684,29 +12721,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12832,7 +12869,9 @@
       <c r="J7" s="14">
         <v>20</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="14">
+        <v>20</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
@@ -12842,11 +12881,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -13069,7 +13108,9 @@
       <c r="J13" s="14">
         <v>20</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="14">
+        <v>20</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -13079,11 +13120,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.38500000000000001</v>
+        <v>0.48499999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -13242,7 +13283,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -13273,7 +13314,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -13305,16 +13346,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.32708333333333334</v>
+        <v>0.41041666666666665</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -13371,7 +13412,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -13396,7 +13437,7 @@
       </c>
       <c r="K21" s="34">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>40.428571428571431</v>
       </c>
       <c r="L21" s="34">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -13446,7 +13487,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>283</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -13496,7 +13537,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -13552,7 +13593,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13577,7 +13618,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -13590,14 +13631,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -13606,15 +13647,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -13623,29 +13664,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -14073,8 +14114,12 @@
       <c r="I15" s="14">
         <v>16</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="14">
+        <v>16</v>
+      </c>
+      <c r="K15" s="14">
+        <v>16</v>
+      </c>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
@@ -14084,11 +14129,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.31578947368421051</v>
+        <v>0.52631578947368418</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -14155,8 +14200,12 @@
       <c r="I17" s="14">
         <v>16</v>
       </c>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="J17" s="14">
+        <v>16</v>
+      </c>
+      <c r="K17" s="14">
+        <v>16</v>
+      </c>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -14166,16 +14215,16 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -14247,7 +14296,7 @@
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -14304,7 +14353,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -14329,7 +14378,7 @@
       </c>
       <c r="K21" s="34">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>54.857142857142854</v>
       </c>
       <c r="L21" s="34">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -14379,7 +14428,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -14429,7 +14478,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -14483,7 +14532,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="20120" topLeftCell="V1"/>
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K14" sqref="K14"/>
       <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -14509,7 +14558,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -14522,14 +14571,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -14538,15 +14587,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -14556,29 +14605,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -14854,7 +14903,9 @@
       <c r="J11" s="14">
         <v>80</v>
       </c>
-      <c r="K11" s="14"/>
+      <c r="K11" s="14">
+        <v>80</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
@@ -14864,11 +14915,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -14938,7 +14989,9 @@
       <c r="J13" s="14">
         <v>80</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="14">
+        <v>80</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
@@ -14948,11 +15001,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -15109,7 +15162,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -15140,7 +15193,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -15172,16 +15225,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -15238,7 +15291,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -15246,7 +15299,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B21" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (C18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -15266,7 +15319,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -15299,7 +15352,7 @@
     </row>
     <row r="22" spans="1:21" hidden="1">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, C18-SUM(G18:G18))</f>
@@ -15319,7 +15372,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -15352,7 +15405,7 @@
     </row>
     <row r="23" spans="1:21" hidden="1">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G23" s="6">
         <f>'Project Summary'!G16</f>
@@ -15372,7 +15425,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -15425,7 +15478,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15450,7 +15503,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -15463,14 +15516,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -15479,15 +15532,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -15496,29 +15549,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -15761,7 +15814,9 @@
       <c r="J10" s="14">
         <v>160</v>
       </c>
-      <c r="K10" s="14"/>
+      <c r="K10" s="14">
+        <v>160</v>
+      </c>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
@@ -15771,11 +15826,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>640</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -16046,7 +16101,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -16077,7 +16132,7 @@
       </c>
       <c r="K18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L18" s="25">
         <f t="shared" si="2"/>
@@ -16109,16 +16164,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>800</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -16175,7 +16230,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -16200,7 +16255,7 @@
       </c>
       <c r="K21" s="6">
         <f>IF(K23 = 0, 0, (C18-SUM(G18:K18))/(MONTH(N1-K5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="L21" s="6">
         <f>IF(L23 = 0, 0, (C18-SUM(G18:L18))/(MONTH(N1-L5)))</f>
@@ -16250,7 +16305,7 @@
       </c>
       <c r="K22" s="6">
         <f>IF(K23=0, 0,C18-SUM(G18:K18))</f>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="L22" s="6">
         <f>IF(L23=0, 0,C18-SUM(G18:L18))</f>
@@ -16300,7 +16355,7 @@
       </c>
       <c r="K23" s="6">
         <f>'Project Summary'!K16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="L23" s="6">
         <f>'Project Summary'!L16</f>
@@ -16340,7 +16395,6 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
effort allocation for January 2010
</commit_message>
<xml_diff>
--- a/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
+++ b/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20700" yWindow="4200" windowWidth="27540" windowHeight="25880" tabRatio="921" activeTab="15"/>
+    <workbookView xWindow="1260" yWindow="-80" windowWidth="24800" windowHeight="16040" tabRatio="921" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Warren" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,10 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
+  <si>
+    <t>Warren Kibbe</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
   <si>
     <t>System Admin</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -365,21 +369,13 @@
   <si>
     <t>Jignesh Patel</t>
   </si>
-  <si>
-    <t>Warren Kibbe</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -562,7 +558,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="105">
@@ -704,21 +700,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -733,7 +729,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1136,7 +1132,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1158,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -1171,35 +1167,35 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
         <v>40344</v>
       </c>
       <c r="Q1" s="94" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R1" s="94"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -1209,32 +1205,32 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -1329,7 +1325,9 @@
       <c r="L6" s="3">
         <v>20</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="3">
+        <v>20</v>
+      </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -1337,11 +1335,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="40">
         <f>SUM(G6:R6)</f>
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="U6" s="4">
         <f>T6/MAX(C6,1)</f>
-        <v>0.47916666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -1656,7 +1654,9 @@
       <c r="L14" s="3">
         <v>8</v>
       </c>
-      <c r="M14" s="3"/>
+      <c r="M14" s="3">
+        <v>8</v>
+      </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -1664,11 +1664,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="40">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="1"/>
-        <v>0.45833333333333331</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1787,7 +1787,7 @@
     </row>
     <row r="18" spans="1:21" hidden="1">
       <c r="A18" s="79" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="79"/>
       <c r="C18" s="79">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="M18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="N18" s="79">
         <f t="shared" si="2"/>
@@ -1850,16 +1850,16 @@
       </c>
       <c r="T18" s="40">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="1"/>
-        <v>0.4375</v>
+        <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="M19" s="4">
         <f xml:space="preserve"> IF(M18=0, 0,(M18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="N19" s="4">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-F18)/F18)</f>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="40">
         <v>192</v>
@@ -1949,11 +1949,11 @@
       </c>
       <c r="M21" s="80">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>37.6</v>
       </c>
       <c r="N21" s="80">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="O21" s="80">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -1999,11 +1999,11 @@
       </c>
       <c r="M22" s="40">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="N22" s="40">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="O22" s="40">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="M23" s="40">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="40">
         <f>'Project Summary'!N16</f>
@@ -2095,7 +2095,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2120,7 +2120,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -2133,14 +2133,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -2149,15 +2149,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -2166,29 +2166,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -2321,7 +2321,9 @@
       <c r="L7" s="14">
         <v>8</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="14">
+        <v>8</v>
+      </c>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -2329,11 +2331,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2716,7 +2718,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -2755,7 +2757,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -2779,16 +2781,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="28" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -2845,7 +2847,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -2878,11 +2880,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -2928,11 +2930,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -2978,7 +2980,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -3023,7 +3025,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3048,7 +3050,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -3061,14 +3063,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -3077,15 +3079,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -3094,29 +3096,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -3248,7 +3250,9 @@
       <c r="L7" s="14">
         <v>12</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="14">
+        <v>12</v>
+      </c>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -3256,11 +3260,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.5546875</v>
+        <v>0.6484375</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3528,7 +3532,9 @@
       <c r="L14" s="14">
         <v>4</v>
       </c>
-      <c r="M14" s="14"/>
+      <c r="M14" s="14">
+        <v>4</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
@@ -3536,11 +3542,11 @@
       <c r="R14" s="14"/>
       <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="1"/>
-        <v>0.390625</v>
+        <v>0.453125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3578,7 +3584,9 @@
       <c r="L15" s="14">
         <v>6</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="14">
+        <v>6</v>
+      </c>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -3586,11 +3594,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.5625</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3628,7 +3636,9 @@
       <c r="L16" s="14">
         <v>6</v>
       </c>
-      <c r="M16" s="14"/>
+      <c r="M16" s="14">
+        <v>6</v>
+      </c>
       <c r="N16" s="14"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14"/>
@@ -3636,11 +3646,11 @@
       <c r="R16" s="14"/>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="1"/>
-        <v>0.5625</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3678,7 +3688,9 @@
       <c r="L17" s="14">
         <v>5</v>
       </c>
-      <c r="M17" s="14"/>
+      <c r="M17" s="14">
+        <v>5</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
@@ -3686,16 +3698,16 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.46875</v>
+        <v>0.546875</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -3734,7 +3746,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -3758,16 +3770,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -3799,7 +3811,7 @@
       </c>
       <c r="M19" s="26">
         <f xml:space="preserve"> IF(M18=0, 0,(M18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="N19" s="26">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-F18)/F18)</f>
@@ -3824,7 +3836,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -3854,11 +3866,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>54.4</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -3904,11 +3916,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>272</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -3954,7 +3966,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -4002,7 +4014,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4027,7 +4039,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -4040,14 +4052,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -4056,15 +4068,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -4074,29 +4086,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -4380,7 +4392,9 @@
       <c r="L11" s="14">
         <v>80</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="14">
+        <v>80</v>
+      </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -4388,11 +4402,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>560</v>
+        <v>640</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>560</v>
+        <v>640</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -4462,7 +4476,9 @@
       <c r="L13" s="14">
         <v>80</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14">
+        <v>80</v>
+      </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -4470,11 +4486,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -4631,7 +4647,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -4670,7 +4686,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -4694,16 +4710,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>1060</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.46875</v>
+        <v>0.55208333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -4760,7 +4776,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1">
       <c r="B20" s="40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -4790,11 +4806,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>255</v>
+        <v>215</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -4840,11 +4856,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>1020</v>
+        <v>860</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -4890,7 +4906,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -4951,11 +4967,11 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="96" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D1" s="96"/>
       <c r="E1" s="96"/>
@@ -4963,13 +4979,13 @@
       <c r="G1" s="96"/>
       <c r="H1" s="96"/>
       <c r="K1" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="42">
         <v>39980</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="42">
         <v>40344</v>
@@ -4977,102 +4993,102 @@
     </row>
     <row r="2" spans="1:20" s="38" customFormat="1">
       <c r="G2" s="38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P2" s="38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S2" s="38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="T2" s="38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="15" customFormat="1">
       <c r="A3" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>77</v>
-      </c>
       <c r="K3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
@@ -5127,7 +5143,7 @@
       </c>
       <c r="M4" s="43">
         <f>Warren!M18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="N4" s="43">
         <f>Warren!N18</f>
@@ -5151,11 +5167,11 @@
       </c>
       <c r="S4" s="88">
         <f t="shared" ref="S4:S15" si="0">SUM(G4:R4)</f>
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="T4" s="28">
         <f>S4/MAX(1,D4)</f>
-        <v>0.4375</v>
+        <v>0.51041666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5208,7 +5224,7 @@
       </c>
       <c r="M5" s="43">
         <f>Sean!M18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N5" s="43">
         <f>Sean!N18</f>
@@ -5232,11 +5248,11 @@
       </c>
       <c r="S5" s="88">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>560</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ref="T5:T16" si="1">S5/MAX(1,D5)</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5289,7 +5305,7 @@
       </c>
       <c r="M6" s="43">
         <f>Rhett!M18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="N6" s="43">
         <f>Rhett!N18</f>
@@ -5313,11 +5329,11 @@
       </c>
       <c r="S6" s="88">
         <f t="shared" si="0"/>
-        <v>768</v>
+        <v>896</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5370,7 +5386,7 @@
       </c>
       <c r="M7" s="43">
         <f>Jalpa!M18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N7" s="43">
         <f>Jalpa!N18</f>
@@ -5451,7 +5467,7 @@
       </c>
       <c r="M8" s="43">
         <f>Nataliya!M18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N8" s="43">
         <f>Nataliya!N18</f>
@@ -5475,11 +5491,11 @@
       </c>
       <c r="S8" s="88">
         <f t="shared" si="0"/>
-        <v>960</v>
+        <v>1120</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5532,7 +5548,7 @@
       </c>
       <c r="M9" s="43">
         <f>John!M18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N9" s="43">
         <f>John!N18</f>
@@ -5613,7 +5629,7 @@
       </c>
       <c r="M10" s="43">
         <f>David!M18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N10" s="43">
         <f>David!N18</f>
@@ -5637,11 +5653,11 @@
       </c>
       <c r="S10" s="88">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>0.49375000000000002</v>
+        <v>0.57708333333333328</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="40" customFormat="1">
@@ -5775,7 +5791,7 @@
       </c>
       <c r="M12" s="43">
         <f>Renee!M18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N12" s="43">
         <f>Renee!N18</f>
@@ -5799,11 +5815,11 @@
       </c>
       <c r="S12" s="88">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5856,7 +5872,7 @@
       </c>
       <c r="M13" s="43">
         <f>Dong!M18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N13" s="43">
         <f>Dong!N18</f>
@@ -5880,11 +5896,11 @@
       </c>
       <c r="S13" s="88">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5937,7 +5953,7 @@
       </c>
       <c r="M14" s="43">
         <f>Lee!M18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N14" s="43">
         <f>Lee!L18</f>
@@ -5961,11 +5977,11 @@
       </c>
       <c r="S14" s="88">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="28">
@@ -6018,7 +6034,7 @@
       </c>
       <c r="M15" s="84">
         <f>'SB-Dev'!M18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N15" s="84">
         <f>'SB-Dev'!N18</f>
@@ -6042,16 +6058,16 @@
       </c>
       <c r="S15" s="88">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>1060</v>
       </c>
       <c r="T15" s="28">
         <f t="shared" si="1"/>
-        <v>0.46875</v>
+        <v>0.55208333333333337</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1">
       <c r="A16" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -6087,7 +6103,7 @@
       </c>
       <c r="M16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N16" s="19">
         <f t="shared" si="2"/>
@@ -6120,7 +6136,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G22" s="30">
         <v>1</v>
@@ -6161,33 +6177,33 @@
     </row>
     <row r="24" spans="1:18" s="76" customFormat="1">
       <c r="A24" s="97" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="98"/>
       <c r="D24" s="76" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" s="76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" s="76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6232,7 +6248,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="45" customFormat="1" ht="14.5" customHeight="1">
       <c r="A1" s="100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="99" t="str">
@@ -6245,14 +6261,14 @@
       <c r="G1" s="85"/>
       <c r="H1" s="85"/>
       <c r="K1" s="47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="86">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="86">
         <f>'Project Summary'!N1</f>
@@ -6271,103 +6287,103 @@
     </row>
     <row r="4" spans="1:21" s="35" customFormat="1">
       <c r="A4" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>34</v>
-      </c>
       <c r="D4" s="35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="35" customFormat="1">
       <c r="A5" s="101"/>
       <c r="G5" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6376,7 +6392,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="83">
         <f>Warren!C6+Sean!C6+Rhett!C6+Jalpa!C6+Nataliya!C6+John!C6+Renee!C6+Dong!C6+Lee!C6+'SB-Dev'!C6</f>
@@ -6416,7 +6432,7 @@
       </c>
       <c r="M6" s="14">
         <f>Warren!M6+Sean!M6+Rhett!M6+Jalpa!M6+Nataliya!M6+John!M6+Renee!M6+Dong!M6+Lee!M6</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N6" s="14">
         <f>Warren!N6+Sean!N6+Rhett!N6+Jalpa!N6+Nataliya!N6+John!N6+Renee!N6+Dong!N6+Lee!N6</f>
@@ -6440,11 +6456,11 @@
       </c>
       <c r="T6">
         <f>SUM(G6:R6)</f>
-        <v>392</v>
+        <v>452</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" ref="U6:U18" si="0">T6/MAX(1,D6)</f>
-        <v>0.58333333333333337</v>
+        <v>0.67261904761904767</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6453,7 +6469,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" s="83">
         <f>Warren!C7+Sean!C7+Rhett!C7+Jalpa!C7+Nataliya!C7+John!C7+Renee!C7+Dong!C7+Lee!C7+'SB-Dev'!C7</f>
@@ -6493,7 +6509,7 @@
       </c>
       <c r="M7" s="14">
         <f>Warren!M7+Sean!M7+Rhett!M7+Jalpa!M7+Nataliya!M7+John!M7+Renee!M7+Dong!M7+Lee!M7</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N7" s="14">
         <f>Warren!N7+Sean!N7+Rhett!N7+Jalpa!N7+Nataliya!N7+John!N7+Renee!N7+Dong!N7+Lee!N7</f>
@@ -6517,11 +6533,11 @@
       </c>
       <c r="T7">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>0.2982456140350877</v>
+        <v>0.32456140350877194</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6530,7 +6546,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="83">
         <f>Warren!C8+Sean!C8+Rhett!C8+Jalpa!C8+Nataliya!C8+John!C8+Renee!C8+Dong!C8+Lee!C8+'SB-Dev'!C8</f>
@@ -6607,7 +6623,7 @@
         <v>3.1</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D9" s="83">
         <f>Warren!C9+Sean!C9+Rhett!C9+Jalpa!C9+Nataliya!C9+John!C9+Renee!C9+Dong!C9+Lee!C9+'SB-Dev'!C9</f>
@@ -6684,7 +6700,7 @@
         <v>3.2</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D10" s="83">
         <f>Warren!C10+Sean!C10+Rhett!C10+Jalpa!C10+Nataliya!C10+John!C10+Renee!C10+Dong!C10+Lee!C10+'SB-Dev'!C10</f>
@@ -6724,7 +6740,7 @@
       </c>
       <c r="M10" s="14">
         <f>Warren!M10+Sean!M10+Rhett!M10+Jalpa!M10+Nataliya!M10+John!M10+Renee!M10+Dong!M10+Lee!M10</f>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="N10" s="14">
         <f>Warren!N10+Sean!N10+Rhett!N10+Jalpa!N10+Nataliya!N10+John!N10+Renee!N10+Dong!N10+Lee!N10</f>
@@ -6748,11 +6764,11 @@
       </c>
       <c r="T10">
         <f t="shared" si="1"/>
-        <v>1620</v>
+        <v>1880</v>
       </c>
       <c r="U10" s="11">
         <f t="shared" si="0"/>
-        <v>1620</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6761,7 +6777,7 @@
         <v>3.3</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="83">
         <f>Warren!C11+Sean!C11+Rhett!C11+Jalpa!C11+Nataliya!C11+John!C11+Renee!C11+Dong!C11+Lee!C11+'SB-Dev'!C11</f>
@@ -6801,7 +6817,7 @@
       </c>
       <c r="M11" s="14">
         <f>Warren!M11+Sean!M11+Rhett!M11+Jalpa!M11+Nataliya!M11+John!M11+Renee!M11+Dong!M11+Lee!M11</f>
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="N11" s="14">
         <f>Warren!N11+Sean!N11+Rhett!N11+Jalpa!N11+Nataliya!N11+John!N11+Renee!N11+Dong!N11+Lee!N11</f>
@@ -6825,11 +6841,11 @@
       </c>
       <c r="T11">
         <f t="shared" si="1"/>
-        <v>780</v>
+        <v>888</v>
       </c>
       <c r="U11" s="11">
         <f t="shared" si="0"/>
-        <v>780</v>
+        <v>888</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="28">
@@ -6838,7 +6854,7 @@
         <v>3.4</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D12" s="83">
         <f>Warren!C12+Sean!C12+Rhett!C12+Jalpa!C12+Nataliya!C12+John!C12+Renee!C12+Dong!C12+Lee!C12+'SB-Dev'!C12</f>
@@ -6878,7 +6894,7 @@
       </c>
       <c r="M12" s="14">
         <f>Warren!M12+Sean!M12+Rhett!M12+Jalpa!M12+Nataliya!M12+John!M12+Renee!M12+Dong!M12+Lee!M12</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N12" s="14">
         <f>Warren!N12+Sean!N12+Rhett!N12+Jalpa!N12+Nataliya!N12+John!N12+Renee!N12+Dong!N12+Lee!N12</f>
@@ -6902,11 +6918,11 @@
       </c>
       <c r="T12">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="U12" s="11">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6914,7 +6930,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="83">
         <f>Warren!C13+Sean!C13+Rhett!C13+Jalpa!C13+Nataliya!C13+John!C13+Renee!C13+Dong!C13+Lee!C13+'SB-Dev'!C13</f>
@@ -6954,7 +6970,7 @@
       </c>
       <c r="M13" s="14">
         <f>Warren!M13+Sean!M13+Rhett!M13+Jalpa!M13+Nataliya!M13+John!M13+Renee!M13+Dong!M13+Lee!M13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="N13" s="14">
         <f>Warren!N13+Sean!N13+Rhett!N13+Jalpa!N13+Nataliya!N13+John!N13+Renee!N13+Dong!N13+Lee!N13</f>
@@ -6978,11 +6994,11 @@
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
-        <v>424</v>
+        <v>508</v>
       </c>
       <c r="U13" s="11">
         <f t="shared" si="0"/>
-        <v>8.8333333333333339</v>
+        <v>10.583333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28">
@@ -6990,7 +7006,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="83">
         <f>Warren!C14+Sean!C14+Rhett!C14+Jalpa!C14+Nataliya!C14+John!C14+Renee!C14+Dong!C14+Lee!C14+'SB-Dev'!C14</f>
@@ -7030,7 +7046,7 @@
       </c>
       <c r="M14" s="14">
         <f>Warren!M14+Sean!M14+Rhett!M14+Jalpa!M14+Nataliya!M14+John!M14+Renee!M14+Dong!M14+Lee!M14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N14" s="14">
         <f>Warren!N14+Sean!N14+Rhett!N14+Jalpa!N14+Nataliya!N14+John!N14+Renee!N14+Dong!N14+Lee!N14</f>
@@ -7054,11 +7070,11 @@
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="0"/>
-        <v>0.251953125</v>
+        <v>0.314453125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -7066,7 +7082,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" s="83">
         <f>Warren!C15+Sean!C15+Rhett!C15+Jalpa!C15+Nataliya!C15+John!C15+Renee!C15+Dong!C15+Lee!C15+'SB-Dev'!C15</f>
@@ -7106,7 +7122,7 @@
       </c>
       <c r="M15" s="14">
         <f>Warren!M15+Sean!M15+Rhett!M15+Jalpa!M15+Nataliya!M15+John!M15+Renee!M15+Dong!M15+Lee!M15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N15" s="14">
         <f>Warren!N15+Sean!N15+Rhett!N15+Jalpa!N15+Nataliya!N15+John!N15+Renee!N15+Dong!N15+Lee!N15</f>
@@ -7130,11 +7146,11 @@
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="0"/>
-        <v>0.1640625</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -7142,7 +7158,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="83">
         <f>Warren!C16+Sean!C16+Rhett!C16+Jalpa!C16+Nataliya!C16+John!C16+Renee!C16+Dong!C16+Lee!C16+'SB-Dev'!C16</f>
@@ -7182,7 +7198,7 @@
       </c>
       <c r="M16" s="14">
         <f>Warren!M16+Sean!M16+Rhett!M16+Jalpa!M16+Nataliya!M16+John!M16+Renee!M16+Dong!M16+Lee!M16</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="N16" s="14">
         <f>Warren!N16+Sean!N16+Rhett!N16+Jalpa!N16+Nataliya!N16+John!N16+Renee!N16+Dong!N16+Lee!N16</f>
@@ -7206,11 +7222,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="1"/>
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="0"/>
-        <v>0.40625</v>
+        <v>0.5223214285714286</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -7218,7 +7234,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="83">
         <f>Warren!C17+Sean!C17+Rhett!C17+Jalpa!C17+Nataliya!C17+John!C17+Renee!C17+Dong!C17+Lee!C17+'SB-Dev'!C17</f>
@@ -7258,7 +7274,7 @@
       </c>
       <c r="M17" s="14">
         <f>Warren!M17+Sean!M17+Rhett!M17+Jalpa!M17+Nataliya!M17+John!M17+Renee!M17+Dong!M17+Lee!M17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N17" s="14">
         <f>Warren!N17+Sean!N17+Rhett!N17+Jalpa!N17+Nataliya!N17+John!N17+Renee!N17+Dong!N17+Lee!N17</f>
@@ -7282,16 +7298,16 @@
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="0"/>
-        <v>0.46875</v>
+        <v>0.546875</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="10" customFormat="1">
       <c r="A18" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -7327,7 +7343,7 @@
       </c>
       <c r="M18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="N18" s="13">
         <f t="shared" si="2"/>
@@ -7352,16 +7368,16 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13">
         <f t="shared" si="1"/>
-        <v>4590</v>
+        <v>5355</v>
       </c>
       <c r="U18" s="12">
         <f t="shared" si="0"/>
-        <v>0.41217672413793105</v>
+        <v>0.48087284482758619</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="4">
@@ -7398,7 +7414,7 @@
       </c>
       <c r="M19" s="26">
         <f xml:space="preserve"> IF(M18=0, 0,(M18-E19)/M18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="N19" s="26">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-E19)/N18)</f>
@@ -7423,7 +7439,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (D18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -7476,7 +7492,7 @@
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, D18-SUM(G18:G18))</f>
@@ -7529,7 +7545,7 @@
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1">
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -8019,15 +8035,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8042,14 +8058,14 @@
       <c r="I1" s="90"/>
       <c r="J1" s="90"/>
       <c r="K1" s="90" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8063,16 +8079,16 @@
     <row r="2" spans="1:18" ht="28">
       <c r="A2" s="90"/>
       <c r="B2" s="90" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="F2" s="90"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -8092,10 +8108,10 @@
     <row r="3" spans="1:18" ht="28">
       <c r="A3" s="90"/>
       <c r="B3" s="90" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="91"/>
       <c r="E3" s="91"/>
@@ -8135,19 +8151,19 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="92" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="92"/>
       <c r="G5" s="81" t="str">
@@ -8235,7 +8251,9 @@
       <c r="L6" s="14">
         <v>16</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="14">
+        <v>16</v>
+      </c>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -8585,7 +8603,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -8624,7 +8642,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="0"/>
@@ -8649,7 +8667,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="90" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" s="90"/>
       <c r="C19" s="26">
@@ -8711,7 +8729,7 @@
     <row r="20" spans="1:18" ht="42">
       <c r="A20" s="6"/>
       <c r="B20" s="90" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -8763,11 +8781,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -8819,11 +8837,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -8875,7 +8893,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -8920,7 +8938,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8945,7 +8963,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8958,14 +8976,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8979,15 +8997,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -8997,10 +9015,10 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -9008,19 +9026,19 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -9114,7 +9132,9 @@
       <c r="L6" s="3">
         <v>50</v>
       </c>
-      <c r="M6" s="3"/>
+      <c r="M6" s="3">
+        <v>40</v>
+      </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -9122,11 +9142,11 @@
       <c r="R6" s="3"/>
       <c r="T6" s="6">
         <f>SUM(G6:R6)</f>
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="U6" s="26">
         <f t="shared" ref="U6:U12" si="0">T6/MAX(C6,1)</f>
-        <v>0.625</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -9438,7 +9458,9 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="3">
+        <v>20</v>
+      </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -9446,11 +9468,11 @@
       <c r="R14" s="3"/>
       <c r="T14" s="6">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="2"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -9522,7 +9544,9 @@
       <c r="L16" s="3">
         <v>20</v>
       </c>
-      <c r="M16" s="3"/>
+      <c r="M16" s="3">
+        <v>20</v>
+      </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -9530,11 +9554,11 @@
       <c r="R16" s="3"/>
       <c r="T16" s="6">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="2"/>
-        <v>0.34375</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -9577,7 +9601,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -9616,7 +9640,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="3"/>
@@ -9640,16 +9664,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>560</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -9706,7 +9730,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -9736,11 +9760,11 @@
       </c>
       <c r="M21" s="34">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -9786,11 +9810,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -9836,7 +9860,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -9881,7 +9905,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9906,7 +9930,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -9919,14 +9943,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
@@ -9935,15 +9959,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -9952,29 +9976,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="22" customFormat="1">
       <c r="A5" s="22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="81" t="str">
@@ -10221,7 +10245,9 @@
       <c r="L10" s="14">
         <v>128</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="14">
+        <v>100</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -10229,11 +10255,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="1"/>
-        <v>640</v>
+        <v>740</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>740</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -10259,7 +10285,9 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="M11" s="14">
+        <v>28</v>
+      </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -10267,11 +10295,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="56">
@@ -10507,7 +10535,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -10546,7 +10574,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="3"/>
@@ -10570,11 +10598,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>768</v>
+        <v>896</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -10633,7 +10661,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1">
         <v>960</v>
@@ -10815,7 +10843,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10840,7 +10868,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -10853,14 +10881,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -10869,15 +10897,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -10886,29 +10914,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -11040,7 +11068,9 @@
       <c r="L7" s="3">
         <v>4</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="3">
+        <v>4</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -11048,11 +11078,11 @@
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -11281,7 +11311,9 @@
       <c r="L13" s="3">
         <v>4</v>
       </c>
-      <c r="M13" s="3"/>
+      <c r="M13" s="3">
+        <v>4</v>
+      </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -11289,11 +11321,11 @@
       <c r="R13" s="3"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -11450,7 +11482,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -11489,7 +11521,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -11513,16 +11545,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -11579,7 +11611,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -11609,11 +11641,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -11659,11 +11691,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -11709,7 +11741,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -11754,7 +11786,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11779,7 +11811,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -11792,14 +11824,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -11808,15 +11840,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -11826,29 +11858,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12176,7 +12208,9 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="M12" s="14">
+        <v>160</v>
+      </c>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -12184,11 +12218,11 @@
       <c r="R12" s="14"/>
       <c r="T12" s="6">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>240</v>
       </c>
       <c r="U12" s="26">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -12383,7 +12417,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -12422,7 +12456,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -12446,16 +12480,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>960</v>
+        <v>1120</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -12512,7 +12546,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -12545,11 +12579,11 @@
       </c>
       <c r="M21" s="34">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -12595,11 +12629,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>960</v>
+        <v>800</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -12645,7 +12679,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -12690,7 +12724,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12715,7 +12749,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -12728,14 +12762,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -12744,15 +12778,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -12761,29 +12795,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12915,7 +12949,9 @@
       <c r="L7" s="14">
         <v>20</v>
       </c>
-      <c r="M7" s="14"/>
+      <c r="M7" s="14">
+        <v>20</v>
+      </c>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -12923,11 +12959,11 @@
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -13156,7 +13192,9 @@
       <c r="L13" s="14">
         <v>20</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14">
+        <v>20</v>
+      </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -13164,11 +13202,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.58499999999999996</v>
+        <v>0.68500000000000005</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -13327,7 +13365,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -13366,7 +13404,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -13390,16 +13428,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.49375000000000002</v>
+        <v>0.57708333333333328</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -13456,7 +13494,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -13489,11 +13527,11 @@
       </c>
       <c r="M21" s="34">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>40.6</v>
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>60.75</v>
+        <v>50.75</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -13539,11 +13577,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>243</v>
+        <v>203</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -13589,7 +13627,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -13637,7 +13675,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13662,7 +13700,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -13675,14 +13713,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -13691,15 +13729,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -13708,29 +13746,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -14167,7 +14205,9 @@
       <c r="L15" s="14">
         <v>16</v>
       </c>
-      <c r="M15" s="14"/>
+      <c r="M15" s="14">
+        <v>16</v>
+      </c>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -14175,11 +14215,11 @@
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.63157894736842102</v>
+        <v>0.73684210526315785</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -14255,7 +14295,9 @@
       <c r="L17" s="14">
         <v>16</v>
       </c>
-      <c r="M17" s="14"/>
+      <c r="M17" s="14">
+        <v>16</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
@@ -14263,16 +14305,16 @@
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -14344,7 +14386,7 @@
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -14401,7 +14443,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -14434,7 +14476,7 @@
       </c>
       <c r="M21" s="34">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>76.8</v>
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
@@ -14484,7 +14526,7 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
@@ -14534,7 +14576,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -14580,7 +14622,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="20120" topLeftCell="V1"/>
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M14" sqref="M14"/>
       <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -14606,7 +14648,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -14619,14 +14661,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -14635,15 +14677,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -14653,29 +14695,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -14957,7 +14999,9 @@
       <c r="L11" s="14">
         <v>80</v>
       </c>
-      <c r="M11" s="14"/>
+      <c r="M11" s="14">
+        <v>80</v>
+      </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -14965,11 +15009,11 @@
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -15045,7 +15089,9 @@
       <c r="L13" s="14">
         <v>80</v>
       </c>
-      <c r="M13" s="14"/>
+      <c r="M13" s="14">
+        <v>80</v>
+      </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -15053,11 +15099,11 @@
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>480</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -15214,7 +15260,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -15253,7 +15299,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -15277,16 +15323,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>960</v>
+        <v>1120</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -15343,7 +15389,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -15351,7 +15397,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B21" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (C18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -15379,11 +15425,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -15404,7 +15450,7 @@
     </row>
     <row r="22" spans="1:21" hidden="1">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, C18-SUM(G18:G18))</f>
@@ -15432,11 +15478,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>960</v>
+        <v>800</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -15457,7 +15503,7 @@
     </row>
     <row r="23" spans="1:21" hidden="1">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="6">
         <f>'Project Summary'!G16</f>
@@ -15485,7 +15531,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
@@ -15530,7 +15576,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15555,7 +15601,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -15568,14 +15614,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -15584,15 +15630,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -15601,29 +15647,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -15872,7 +15918,9 @@
       <c r="L10" s="14">
         <v>160</v>
       </c>
-      <c r="M10" s="14"/>
+      <c r="M10" s="14">
+        <v>160</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -15880,11 +15928,11 @@
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>960</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>960</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -16155,7 +16203,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -16194,7 +16242,7 @@
       </c>
       <c r="M18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
@@ -16218,16 +16266,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>960</v>
+        <v>1120</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -16284,7 +16332,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -16317,11 +16365,11 @@
       </c>
       <c r="M21" s="6">
         <f>IF(M23 = 0, 0, (C18-SUM(G18:M18))/(MONTH(N1-M5)))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
@@ -16367,11 +16415,11 @@
       </c>
       <c r="M22" s="6">
         <f>IF(M23=0, 0,C18-SUM(G18:M18))</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>960</v>
+        <v>800</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
@@ -16417,7 +16465,7 @@
       </c>
       <c r="M23" s="6">
         <f>'Project Summary'!M16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>

</xml_diff>

<commit_message>
monthly status effort report
</commit_message>
<xml_diff>
--- a/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
+++ b/deliverables/trunk/studycalendar/PhaseIV/MSR_LOE_PSC2009.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="-80" windowWidth="24800" windowHeight="16040" tabRatio="921" activeTab="15"/>
+    <workbookView xWindow="-80" yWindow="-2180" windowWidth="28760" windowHeight="18200" tabRatio="921" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Warren" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="109">
+  <si>
+    <t>Jignesh Patel</t>
+  </si>
   <si>
     <t>Warren Kibbe</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -365,9 +368,6 @@
   </si>
   <si>
     <t>David Patton</t>
-  </si>
-  <si>
-    <t>Jignesh Patel</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1132,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1154,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -1167,35 +1167,35 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
         <v>40344</v>
       </c>
       <c r="Q1" s="94" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="R1" s="94"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -1205,32 +1205,32 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -1328,18 +1328,24 @@
       <c r="M6" s="3">
         <v>20</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="N6" s="3">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3">
+        <v>20</v>
+      </c>
+      <c r="P6" s="3">
+        <v>20</v>
+      </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="T6" s="40">
         <f>SUM(G6:R6)</f>
-        <v>112</v>
+        <v>172</v>
       </c>
       <c r="U6" s="4">
         <f>T6/MAX(C6,1)</f>
-        <v>0.58333333333333337</v>
+        <v>0.89583333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -1657,18 +1663,24 @@
       <c r="M14" s="3">
         <v>8</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="N14" s="3">
+        <v>8</v>
+      </c>
+      <c r="O14" s="3">
+        <v>8</v>
+      </c>
+      <c r="P14" s="3">
+        <v>8</v>
+      </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="T14" s="40">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="1"/>
-        <v>0.54166666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1787,7 +1799,7 @@
     </row>
     <row r="18" spans="1:21" hidden="1">
       <c r="A18" s="79" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="79"/>
       <c r="C18" s="79">
@@ -1830,15 +1842,15 @@
       </c>
       <c r="N18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="O18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P18" s="79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="Q18" s="79">
         <f t="shared" si="2"/>
@@ -1850,16 +1862,16 @@
       </c>
       <c r="T18" s="40">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>280</v>
       </c>
       <c r="U18" s="4">
         <f t="shared" si="1"/>
-        <v>0.51041666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -1895,15 +1907,15 @@
       </c>
       <c r="N19" s="4">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="O19" s="4">
         <f xml:space="preserve"> IF(O18=0, 0,(O18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="P19" s="4">
         <f xml:space="preserve"> IF(P18=0, 0,(P18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.125</v>
       </c>
       <c r="Q19" s="4">
         <f xml:space="preserve"> IF(Q18=0, 0,(Q18-F18)/F18)</f>
@@ -1916,7 +1928,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="40">
         <v>192</v>
@@ -1953,15 +1965,15 @@
       </c>
       <c r="N21" s="80">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="O21" s="80">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="P21" s="80">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>34.666666666666664</v>
       </c>
       <c r="Q21" s="80">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -2003,15 +2015,15 @@
       </c>
       <c r="N22" s="40">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="O22" s="40">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="P22" s="40">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="Q22" s="40">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -2053,15 +2065,15 @@
       </c>
       <c r="N23" s="40">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="40">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="40">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="40">
         <f>'Project Summary'!Q16</f>
@@ -2095,7 +2107,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2120,7 +2132,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -2133,14 +2145,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -2149,15 +2161,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -2166,29 +2178,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -2324,18 +2336,24 @@
       <c r="M7" s="14">
         <v>8</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="N7" s="14">
+        <v>8</v>
+      </c>
+      <c r="O7" s="14">
+        <v>8</v>
+      </c>
+      <c r="P7" s="14">
+        <v>8</v>
+      </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2718,7 +2736,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -2761,15 +2779,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -2781,16 +2799,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="28" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="4">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -2847,7 +2865,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -2884,15 +2902,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -2934,15 +2952,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -2984,15 +3002,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -3022,10 +3040,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -3050,7 +3071,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -3063,14 +3084,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -3079,15 +3100,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -3096,29 +3117,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -3253,18 +3274,24 @@
       <c r="M7" s="14">
         <v>12</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="N7" s="14">
+        <v>12</v>
+      </c>
+      <c r="O7" s="14">
+        <v>12</v>
+      </c>
+      <c r="P7" s="14">
+        <v>12</v>
+      </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.6484375</v>
+        <v>0.9296875</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3535,18 +3562,24 @@
       <c r="M14" s="14">
         <v>4</v>
       </c>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="N14" s="14">
+        <v>4</v>
+      </c>
+      <c r="O14" s="14">
+        <v>4</v>
+      </c>
+      <c r="P14" s="14">
+        <v>4</v>
+      </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="14"/>
       <c r="T14" s="6">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="1"/>
-        <v>0.453125</v>
+        <v>0.640625</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3587,18 +3620,24 @@
       <c r="M15" s="14">
         <v>6</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="N15" s="14">
+        <v>6</v>
+      </c>
+      <c r="O15" s="14">
+        <v>6</v>
+      </c>
+      <c r="P15" s="14">
+        <v>6</v>
+      </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.65625</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3639,18 +3678,24 @@
       <c r="M16" s="14">
         <v>6</v>
       </c>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
+      <c r="N16" s="14">
+        <v>6</v>
+      </c>
+      <c r="O16" s="14">
+        <v>6</v>
+      </c>
+      <c r="P16" s="14">
+        <v>6</v>
+      </c>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
       <c r="T16" s="6">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="1"/>
-        <v>0.65625</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3691,23 +3736,29 @@
       <c r="M17" s="14">
         <v>5</v>
       </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
+      <c r="N17" s="14">
+        <v>5</v>
+      </c>
+      <c r="O17" s="14">
+        <v>5</v>
+      </c>
+      <c r="P17" s="14">
+        <v>5</v>
+      </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.546875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -3750,15 +3801,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -3770,16 +3821,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -3815,15 +3866,15 @@
       </c>
       <c r="N19" s="26">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="O19" s="26">
         <f xml:space="preserve"> IF(O18=0, 0,(O18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="P19" s="26">
         <f xml:space="preserve"> IF(P18=0, 0,(P18-F18)/F18)</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Q19" s="26">
         <f xml:space="preserve"> IF(Q18=0, 0,(Q18-F18)/F18)</f>
@@ -3836,7 +3887,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -3870,15 +3921,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>74.666666666666671</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -3920,15 +3971,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>224</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -3970,15 +4021,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -3998,12 +4049,13 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="C18" formulaRange="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
@@ -4014,7 +4066,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4039,7 +4091,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -4052,14 +4104,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -4068,15 +4120,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -4086,29 +4138,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -4395,18 +4447,24 @@
       <c r="M11" s="14">
         <v>80</v>
       </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="N11" s="14">
+        <v>80</v>
+      </c>
+      <c r="O11" s="14">
+        <v>80</v>
+      </c>
+      <c r="P11" s="14">
+        <v>80</v>
+      </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>880</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>640</v>
+        <v>880</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -4479,18 +4537,24 @@
       <c r="M13" s="14">
         <v>80</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
+      <c r="N13" s="14">
+        <v>80</v>
+      </c>
+      <c r="O13" s="14">
+        <v>80</v>
+      </c>
+      <c r="P13" s="14">
+        <v>80</v>
+      </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>560</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>560</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -4647,7 +4711,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -4690,15 +4754,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -4710,16 +4774,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>1060</v>
+        <v>1540</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.55208333333333337</v>
+        <v>0.80208333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -4776,7 +4840,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1">
       <c r="B20" s="40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -4810,15 +4874,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>126.66666666666667</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -4860,15 +4924,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>860</v>
+        <v>700</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>380</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -4910,15 +4974,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -4967,11 +5031,11 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="96" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D1" s="96"/>
       <c r="E1" s="96"/>
@@ -4979,13 +5043,13 @@
       <c r="G1" s="96"/>
       <c r="H1" s="96"/>
       <c r="K1" s="30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="42">
         <v>39980</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="42">
         <v>40344</v>
@@ -4993,102 +5057,102 @@
     </row>
     <row r="2" spans="1:20" s="38" customFormat="1">
       <c r="G2" s="38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P2" s="38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="38" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S2" s="38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="T2" s="38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="15" customFormat="1">
       <c r="A3" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="K3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="Q3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>82</v>
       </c>
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
@@ -5147,15 +5211,15 @@
       </c>
       <c r="N4" s="43">
         <f>Warren!N18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="O4" s="43">
         <f>Warren!O18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P4" s="77">
         <f>Warren!P18</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="77">
         <f>Warren!Q18</f>
@@ -5167,11 +5231,11 @@
       </c>
       <c r="S4" s="88">
         <f t="shared" ref="S4:S15" si="0">SUM(G4:R4)</f>
-        <v>196</v>
+        <v>280</v>
       </c>
       <c r="T4" s="28">
         <f>S4/MAX(1,D4)</f>
-        <v>0.51041666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -5228,7 +5292,7 @@
       </c>
       <c r="N5" s="43">
         <f>Sean!N18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="O5" s="43">
         <f>Sean!O19</f>
@@ -5236,7 +5300,7 @@
       </c>
       <c r="P5" s="77">
         <f>Sean!P18</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="77">
         <f>Sean!Q18</f>
@@ -5248,11 +5312,11 @@
       </c>
       <c r="S5" s="88">
         <f t="shared" si="0"/>
-        <v>560</v>
+        <v>720</v>
       </c>
       <c r="T5" s="28">
         <f t="shared" ref="T5:T16" si="1">S5/MAX(1,D5)</f>
-        <v>0.58333333333333337</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -5309,15 +5373,15 @@
       </c>
       <c r="N6" s="43">
         <f>Rhett!N18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="O6" s="43">
         <f>Rhett!O18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="P6" s="77">
         <f>Rhett!P18</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="Q6" s="77">
         <f>Rhett!Q18</f>
@@ -5329,11 +5393,11 @@
       </c>
       <c r="S6" s="88">
         <f t="shared" si="0"/>
-        <v>896</v>
+        <v>1280</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -5390,15 +5454,15 @@
       </c>
       <c r="N7" s="43">
         <f>Jalpa!N18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O7" s="43">
         <f>Nataliya!O18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P7" s="77">
         <f>Jalpa!P18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q7" s="77">
         <f>Jalpa!Q18</f>
@@ -5471,15 +5535,15 @@
       </c>
       <c r="N8" s="43">
         <f>Nataliya!N18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O8" s="43">
         <f>Nataliya!O18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P8" s="77">
         <f>Nataliya!P18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q8" s="77">
         <f>Nataliya!Q18</f>
@@ -5491,11 +5555,11 @@
       </c>
       <c r="S8" s="88">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1600</v>
       </c>
       <c r="T8" s="28">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -5552,15 +5616,15 @@
       </c>
       <c r="N9" s="43">
         <f>John!N18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O9" s="43">
         <f>John!O18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P9" s="77">
         <f>John!P18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q9" s="77">
         <f>John!Q18</f>
@@ -5633,15 +5697,15 @@
       </c>
       <c r="N10" s="43">
         <f>David!N18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O10" s="43">
         <f>David!O18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P10" s="43">
         <f>David!P18</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="43">
         <f>David!Q18</f>
@@ -5653,11 +5717,11 @@
       </c>
       <c r="S10" s="88">
         <f t="shared" si="0"/>
-        <v>277</v>
+        <v>397</v>
       </c>
       <c r="T10" s="28">
         <f t="shared" si="1"/>
-        <v>0.57708333333333328</v>
+        <v>0.82708333333333328</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="40" customFormat="1">
@@ -5795,15 +5859,15 @@
       </c>
       <c r="N12" s="43">
         <f>Renee!N18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O12" s="43">
         <f>Renee!O18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P12" s="77">
         <f>Renee!P18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q12" s="77">
         <f>Renee!Q18</f>
@@ -5815,11 +5879,11 @@
       </c>
       <c r="S12" s="88">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="T12" s="28">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -5876,15 +5940,15 @@
       </c>
       <c r="N13" s="43">
         <f>Dong!N18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O13" s="43">
         <f>Dong!O18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P13" s="77">
         <f>Dong!P18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q13" s="77">
         <f>Dong!Q18</f>
@@ -5896,11 +5960,11 @@
       </c>
       <c r="S13" s="88">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="T13" s="28">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -5961,11 +6025,11 @@
       </c>
       <c r="O14" s="43">
         <f>Lee!O18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P14" s="77">
         <f>Lee!P18</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q14" s="77">
         <f>Lee!Q18</f>
@@ -5977,11 +6041,11 @@
       </c>
       <c r="S14" s="88">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="T14" s="28">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="28">
@@ -6038,15 +6102,15 @@
       </c>
       <c r="N15" s="84">
         <f>'SB-Dev'!N18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O15" s="84">
         <f>'SB-Dev'!O18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P15" s="84">
         <f>'SB-Dev'!P18</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q15" s="84">
         <f>'SB-Dev'!Q18</f>
@@ -6058,16 +6122,16 @@
       </c>
       <c r="S15" s="88">
         <f t="shared" si="0"/>
-        <v>1060</v>
+        <v>1540</v>
       </c>
       <c r="T15" s="28">
         <f t="shared" si="1"/>
-        <v>0.55208333333333337</v>
+        <v>0.80208333333333337</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="6" customFormat="1">
       <c r="A16" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -6107,15 +6171,15 @@
       </c>
       <c r="N16" s="19">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q16" s="19">
         <f t="shared" si="2"/>
@@ -6136,7 +6200,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G22" s="30">
         <v>1</v>
@@ -6177,33 +6241,33 @@
     </row>
     <row r="24" spans="1:18" s="76" customFormat="1">
       <c r="A24" s="97" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B24" s="98"/>
       <c r="D24" s="76" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24" s="76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="76" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -6248,7 +6312,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="45" customFormat="1" ht="14.5" customHeight="1">
       <c r="A1" s="100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="100"/>
       <c r="C1" s="99" t="str">
@@ -6261,14 +6325,14 @@
       <c r="G1" s="85"/>
       <c r="H1" s="85"/>
       <c r="K1" s="47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="86">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="86">
         <f>'Project Summary'!N1</f>
@@ -6287,103 +6351,103 @@
     </row>
     <row r="4" spans="1:21" s="35" customFormat="1">
       <c r="A4" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>35</v>
-      </c>
       <c r="D4" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P4" s="35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R4" s="35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T4" s="35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="35" customFormat="1">
       <c r="A5" s="101"/>
       <c r="G5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -6392,7 +6456,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="83">
         <f>Warren!C6+Sean!C6+Rhett!C6+Jalpa!C6+Nataliya!C6+John!C6+Renee!C6+Dong!C6+Lee!C6+'SB-Dev'!C6</f>
@@ -6436,15 +6500,15 @@
       </c>
       <c r="N6" s="14">
         <f>Warren!N6+Sean!N6+Rhett!N6+Jalpa!N6+Nataliya!N6+John!N6+Renee!N6+Dong!N6+Lee!N6</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="O6" s="14">
         <f>Warren!O6+Sean!O6+Rhett!O6+Jalpa!O6+Nataliya!O6+John!O6+Renee!O6+Dong!O6+Lee!O6</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P6" s="14">
         <f>Warren!P6+Sean!P6+Rhett!P6+Jalpa!P6+Nataliya!P6+John!P6+Renee!P6+Dong!P6+Lee!P6</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q6" s="14">
         <f>Warren!Q6+Sean!Q6+Rhett!Q6+Jalpa!Q6+Nataliya!Q6+John!Q6+Renee!Q6+Dong!Q6+Lee!Q6</f>
@@ -6456,11 +6520,11 @@
       </c>
       <c r="T6">
         <f>SUM(G6:R6)</f>
-        <v>452</v>
+        <v>632</v>
       </c>
       <c r="U6" s="11">
         <f t="shared" ref="U6:U18" si="0">T6/MAX(1,D6)</f>
-        <v>0.67261904761904767</v>
+        <v>0.94047619047619047</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -6469,7 +6533,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="83">
         <f>Warren!C7+Sean!C7+Rhett!C7+Jalpa!C7+Nataliya!C7+John!C7+Renee!C7+Dong!C7+Lee!C7+'SB-Dev'!C7</f>
@@ -6513,15 +6577,15 @@
       </c>
       <c r="N7" s="14">
         <f>Warren!N7+Sean!N7+Rhett!N7+Jalpa!N7+Nataliya!N7+John!N7+Renee!N7+Dong!N7+Lee!N7</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="O7" s="14">
         <f>Warren!O7+Sean!O7+Rhett!O7+Jalpa!O7+Nataliya!O7+John!O7+Renee!O7+Dong!O7+Lee!O7</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="P7" s="14">
         <f>Warren!P7+Sean!P7+Rhett!P7+Jalpa!P7+Nataliya!P7+John!P7+Renee!P7+Dong!P7+Lee!P7</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q7" s="14">
         <f>Warren!Q7+Sean!Q7+Rhett!Q7+Jalpa!Q7+Nataliya!Q7+John!Q7+Renee!Q7+Dong!Q7+Lee!Q7</f>
@@ -6533,11 +6597,11 @@
       </c>
       <c r="T7">
         <f t="shared" ref="T7:T18" si="1">SUM(G7:R7)</f>
-        <v>296</v>
+        <v>368</v>
       </c>
       <c r="U7" s="11">
         <f t="shared" si="0"/>
-        <v>0.32456140350877194</v>
+        <v>0.40350877192982454</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -6546,7 +6610,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="83">
         <f>Warren!C8+Sean!C8+Rhett!C8+Jalpa!C8+Nataliya!C8+John!C8+Renee!C8+Dong!C8+Lee!C8+'SB-Dev'!C8</f>
@@ -6623,7 +6687,7 @@
         <v>3.1</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" s="83">
         <f>Warren!C9+Sean!C9+Rhett!C9+Jalpa!C9+Nataliya!C9+John!C9+Renee!C9+Dong!C9+Lee!C9+'SB-Dev'!C9</f>
@@ -6700,7 +6764,7 @@
         <v>3.2</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" s="83">
         <f>Warren!C10+Sean!C10+Rhett!C10+Jalpa!C10+Nataliya!C10+John!C10+Renee!C10+Dong!C10+Lee!C10+'SB-Dev'!C10</f>
@@ -6744,15 +6808,15 @@
       </c>
       <c r="N10" s="14">
         <f>Warren!N10+Sean!N10+Rhett!N10+Jalpa!N10+Nataliya!N10+John!N10+Renee!N10+Dong!N10+Lee!N10</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="O10" s="14">
         <f>Warren!O10+Sean!O10+Rhett!O10+Jalpa!O10+Nataliya!O10+John!O10+Renee!O10+Dong!O10+Lee!O10</f>
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="P10" s="14">
         <f>Warren!P10+Sean!P10+Rhett!P10+Jalpa!P10+Nataliya!P10+John!P10+Renee!P10+Dong!P10+Lee!P10</f>
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="Q10" s="14">
         <f>Warren!Q10+Sean!Q10+Rhett!Q10+Jalpa!Q10+Nataliya!Q10+John!Q10+Renee!Q10+Dong!Q10+Lee!Q10</f>
@@ -6764,11 +6828,11 @@
       </c>
       <c r="T10">
         <f t="shared" si="1"/>
-        <v>1880</v>
+        <v>2560</v>
       </c>
       <c r="U10" s="11">
         <f t="shared" si="0"/>
-        <v>1880</v>
+        <v>2560</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -6777,7 +6841,7 @@
         <v>3.3</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" s="83">
         <f>Warren!C11+Sean!C11+Rhett!C11+Jalpa!C11+Nataliya!C11+John!C11+Renee!C11+Dong!C11+Lee!C11+'SB-Dev'!C11</f>
@@ -6821,15 +6885,15 @@
       </c>
       <c r="N11" s="14">
         <f>Warren!N11+Sean!N11+Rhett!N11+Jalpa!N11+Nataliya!N11+John!N11+Renee!N11+Dong!N11+Lee!N11</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="O11" s="14">
         <f>Warren!O11+Sean!O11+Rhett!O11+Jalpa!O11+Nataliya!O11+John!O11+Renee!O11+Dong!O11+Lee!O11</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="P11" s="14">
         <f>Warren!P11+Sean!P11+Rhett!P11+Jalpa!P11+Nataliya!P11+John!P11+Renee!P11+Dong!P11+Lee!P11</f>
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="Q11" s="14">
         <f>Warren!Q11+Sean!Q11+Rhett!Q11+Jalpa!Q11+Nataliya!Q11+John!Q11+Renee!Q11+Dong!Q11+Lee!Q11</f>
@@ -6841,11 +6905,11 @@
       </c>
       <c r="T11">
         <f t="shared" si="1"/>
-        <v>888</v>
+        <v>1312</v>
       </c>
       <c r="U11" s="11">
         <f t="shared" si="0"/>
-        <v>888</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="28">
@@ -6854,7 +6918,7 @@
         <v>3.4</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D12" s="83">
         <f>Warren!C12+Sean!C12+Rhett!C12+Jalpa!C12+Nataliya!C12+John!C12+Renee!C12+Dong!C12+Lee!C12+'SB-Dev'!C12</f>
@@ -6898,15 +6962,15 @@
       </c>
       <c r="N12" s="14">
         <f>Warren!N12+Sean!N12+Rhett!N12+Jalpa!N12+Nataliya!N12+John!N12+Renee!N12+Dong!N12+Lee!N12</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O12" s="14">
         <f>Warren!O12+Sean!O12+Rhett!O12+Jalpa!O12+Nataliya!O12+John!O12+Renee!O12+Dong!O12+Lee!O12</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P12" s="14">
         <f>Warren!P12+Sean!P12+Rhett!P12+Jalpa!P12+Nataliya!P12+John!P12+Renee!P12+Dong!P12+Lee!P12</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q12" s="14">
         <f>Warren!Q12+Sean!Q12+Rhett!Q12+Jalpa!Q12+Nataliya!Q12+John!Q12+Renee!Q12+Dong!Q12+Lee!Q12</f>
@@ -6918,11 +6982,11 @@
       </c>
       <c r="T12">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>800</v>
       </c>
       <c r="U12" s="11">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>800</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -6930,7 +6994,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="83">
         <f>Warren!C13+Sean!C13+Rhett!C13+Jalpa!C13+Nataliya!C13+John!C13+Renee!C13+Dong!C13+Lee!C13+'SB-Dev'!C13</f>
@@ -6974,15 +7038,15 @@
       </c>
       <c r="N13" s="14">
         <f>Warren!N13+Sean!N13+Rhett!N13+Jalpa!N13+Nataliya!N13+John!N13+Renee!N13+Dong!N13+Lee!N13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="O13" s="14">
         <f>Warren!O13+Sean!O13+Rhett!O13+Jalpa!O13+Nataliya!O13+John!O13+Renee!O13+Dong!O13+Lee!O13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="P13" s="14">
         <f>Warren!P13+Sean!P13+Rhett!P13+Jalpa!P13+Nataliya!P13+John!P13+Renee!P13+Dong!P13+Lee!P13</f>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="Q13" s="14">
         <f>Warren!Q13+Sean!Q13+Rhett!Q13+Jalpa!Q13+Nataliya!Q13+John!Q13+Renee!Q13+Dong!Q13+Lee!Q13</f>
@@ -6994,11 +7058,11 @@
       </c>
       <c r="T13">
         <f t="shared" si="1"/>
-        <v>508</v>
+        <v>760</v>
       </c>
       <c r="U13" s="11">
         <f t="shared" si="0"/>
-        <v>10.583333333333334</v>
+        <v>15.833333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="28">
@@ -7006,7 +7070,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="83">
         <f>Warren!C14+Sean!C14+Rhett!C14+Jalpa!C14+Nataliya!C14+John!C14+Renee!C14+Dong!C14+Lee!C14+'SB-Dev'!C14</f>
@@ -7050,15 +7114,15 @@
       </c>
       <c r="N14" s="14">
         <f>Warren!N14+Sean!N14+Rhett!N14+Jalpa!N14+Nataliya!N14+John!N14+Renee!N14+Dong!N14+Lee!N14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O14" s="14">
         <f>Warren!O14+Sean!O14+Rhett!O14+Jalpa!O14+Nataliya!O14+John!O14+Renee!O14+Dong!O14+Lee!O14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="P14" s="14">
         <f>Warren!P14+Sean!P14+Rhett!P14+Jalpa!P14+Nataliya!P14+John!P14+Renee!P14+Dong!P14+Lee!P14</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="Q14" s="14">
         <f>Warren!Q14+Sean!Q14+Rhett!Q14+Jalpa!Q14+Nataliya!Q14+John!Q14+Renee!Q14+Dong!Q14+Lee!Q14</f>
@@ -7070,11 +7134,11 @@
       </c>
       <c r="T14">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>257</v>
       </c>
       <c r="U14" s="11">
         <f t="shared" si="0"/>
-        <v>0.314453125</v>
+        <v>0.501953125</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -7082,7 +7146,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="83">
         <f>Warren!C15+Sean!C15+Rhett!C15+Jalpa!C15+Nataliya!C15+John!C15+Renee!C15+Dong!C15+Lee!C15+'SB-Dev'!C15</f>
@@ -7126,15 +7190,15 @@
       </c>
       <c r="N15" s="14">
         <f>Warren!N15+Sean!N15+Rhett!N15+Jalpa!N15+Nataliya!N15+John!N15+Renee!N15+Dong!N15+Lee!N15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O15" s="14">
         <f>Warren!O15+Sean!O15+Rhett!O15+Jalpa!O15+Nataliya!O15+John!O15+Renee!O15+Dong!O15+Lee!O15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P15" s="14">
         <f>Warren!P15+Sean!P15+Rhett!P15+Jalpa!P15+Nataliya!P15+John!P15+Renee!P15+Dong!P15+Lee!P15</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q15" s="14">
         <f>Warren!Q15+Sean!Q15+Rhett!Q15+Jalpa!Q15+Nataliya!Q15+John!Q15+Renee!Q15+Dong!Q15+Lee!Q15</f>
@@ -7146,11 +7210,11 @@
       </c>
       <c r="T15">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="U15" s="11">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>0.2578125</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -7158,7 +7222,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="83">
         <f>Warren!C16+Sean!C16+Rhett!C16+Jalpa!C16+Nataliya!C16+John!C16+Renee!C16+Dong!C16+Lee!C16+'SB-Dev'!C16</f>
@@ -7202,15 +7266,15 @@
       </c>
       <c r="N16" s="14">
         <f>Warren!N16+Sean!N16+Rhett!N16+Jalpa!N16+Nataliya!N16+John!N16+Renee!N16+Dong!N16+Lee!N16</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="O16" s="14">
         <f>Warren!O16+Sean!O16+Rhett!O16+Jalpa!O16+Nataliya!O16+John!O16+Renee!O16+Dong!O16+Lee!O16</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="P16" s="14">
         <f>Warren!P16+Sean!P16+Rhett!P16+Jalpa!P16+Nataliya!P16+John!P16+Renee!P16+Dong!P16+Lee!P16</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Q16" s="14">
         <f>Warren!Q16+Sean!Q16+Rhett!Q16+Jalpa!Q16+Nataliya!Q16+John!Q16+Renee!Q16+Dong!Q16+Lee!Q16</f>
@@ -7222,11 +7286,11 @@
       </c>
       <c r="T16">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="U16" s="11">
         <f t="shared" si="0"/>
-        <v>0.5223214285714286</v>
+        <v>0.8705357142857143</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -7234,7 +7298,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="83">
         <f>Warren!C17+Sean!C17+Rhett!C17+Jalpa!C17+Nataliya!C17+John!C17+Renee!C17+Dong!C17+Lee!C17+'SB-Dev'!C17</f>
@@ -7278,15 +7342,15 @@
       </c>
       <c r="N17" s="14">
         <f>Warren!N17+Sean!N17+Rhett!N17+Jalpa!N17+Nataliya!N17+John!N17+Renee!N17+Dong!N17+Lee!N17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O17" s="14">
         <f>Warren!O17+Sean!O17+Rhett!O17+Jalpa!O17+Nataliya!O17+John!O17+Renee!O17+Dong!O17+Lee!O17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P17" s="14">
         <f>Warren!P17+Sean!P17+Rhett!P17+Jalpa!P17+Nataliya!P17+John!P17+Renee!P17+Dong!P17+Lee!P17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="14">
         <f>Warren!Q17+Sean!Q17+Rhett!Q17+Jalpa!Q17+Nataliya!Q17+John!Q17+Renee!Q17+Dong!Q17+Lee!Q17</f>
@@ -7298,16 +7362,16 @@
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="U17" s="11">
         <f t="shared" si="0"/>
-        <v>0.546875</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="10" customFormat="1">
       <c r="A18" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -7347,15 +7411,15 @@
       </c>
       <c r="N18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="P18" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>765</v>
       </c>
       <c r="Q18" s="13">
         <f t="shared" si="2"/>
@@ -7368,16 +7432,16 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13">
         <f t="shared" si="1"/>
-        <v>5355</v>
+        <v>7650</v>
       </c>
       <c r="U18" s="12">
         <f t="shared" si="0"/>
-        <v>0.48087284482758619</v>
+        <v>0.68696120689655171</v>
       </c>
     </row>
     <row r="19" spans="1:21" s="4" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26"/>
       <c r="D19" s="4">
@@ -7418,15 +7482,15 @@
       </c>
       <c r="N19" s="26">
         <f xml:space="preserve"> IF(N18=0, 0,(N18-E19)/N18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="O19" s="26">
         <f xml:space="preserve"> IF(O18=0, 0,(O18-E19)/O18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="P19" s="26">
         <f xml:space="preserve"> IF(P18=0, 0,(P18-E19)/P18)</f>
-        <v>0</v>
+        <v>-0.21307189542483659</v>
       </c>
       <c r="Q19" s="26">
         <f xml:space="preserve"> IF(Q18=0, 0,(Q18-E19)/Q18)</f>
@@ -7439,7 +7503,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1">
       <c r="A21" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (D18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -7492,7 +7556,7 @@
     </row>
     <row r="22" spans="1:21" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, D18-SUM(G18:G18))</f>
@@ -7545,7 +7609,7 @@
     </row>
     <row r="23" spans="1:21" s="1" customFormat="1">
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -8036,14 +8100,14 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8058,14 +8122,14 @@
       <c r="I1" s="90"/>
       <c r="J1" s="90"/>
       <c r="K1" s="90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="90" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8079,16 +8143,16 @@
     <row r="2" spans="1:18" ht="28">
       <c r="A2" s="90"/>
       <c r="B2" s="90" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="F2" s="90"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -8108,10 +8172,10 @@
     <row r="3" spans="1:18" ht="28">
       <c r="A3" s="90"/>
       <c r="B3" s="90" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="91"/>
       <c r="E3" s="91"/>
@@ -8151,19 +8215,19 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="92" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="92"/>
       <c r="G5" s="81" t="str">
@@ -8254,9 +8318,15 @@
       <c r="M6" s="14">
         <v>16</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="N6" s="14">
+        <v>16</v>
+      </c>
+      <c r="O6" s="14">
+        <v>16</v>
+      </c>
+      <c r="P6" s="14">
+        <v>16</v>
+      </c>
       <c r="Q6" s="14"/>
       <c r="R6" s="14"/>
     </row>
@@ -8603,7 +8673,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -8646,15 +8716,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="0"/>
@@ -8667,7 +8737,7 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="90" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B19" s="90"/>
       <c r="C19" s="26">
@@ -8729,7 +8799,7 @@
     <row r="20" spans="1:18" ht="42">
       <c r="A20" s="6"/>
       <c r="B20" s="90" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -8785,15 +8855,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -8841,15 +8911,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -8897,15 +8967,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -8938,7 +9008,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8963,7 +9033,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -8976,14 +9046,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -8997,15 +9067,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -9015,10 +9085,10 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -9026,19 +9096,19 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -9135,18 +9205,24 @@
       <c r="M6" s="3">
         <v>40</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+      <c r="N6" s="3">
+        <v>40</v>
+      </c>
+      <c r="O6" s="3">
+        <v>40</v>
+      </c>
+      <c r="P6" s="3">
+        <v>40</v>
+      </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="T6" s="6">
         <f>SUM(G6:R6)</f>
-        <v>340</v>
+        <v>460</v>
       </c>
       <c r="U6" s="26">
         <f t="shared" ref="U6:U12" si="0">T6/MAX(C6,1)</f>
-        <v>0.70833333333333337</v>
+        <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="28">
@@ -9461,18 +9537,24 @@
       <c r="M14" s="3">
         <v>20</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="N14" s="3">
+        <v>20</v>
+      </c>
+      <c r="O14" s="3">
+        <v>20</v>
+      </c>
+      <c r="P14" s="3">
+        <v>20</v>
+      </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="T14" s="6">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="U14" s="26">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -9547,18 +9629,24 @@
       <c r="M16" s="3">
         <v>20</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+      <c r="N16" s="3">
+        <v>20</v>
+      </c>
+      <c r="O16" s="3">
+        <v>20</v>
+      </c>
+      <c r="P16" s="3">
+        <v>20</v>
+      </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="T16" s="6">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="U16" s="26">
         <f t="shared" si="2"/>
-        <v>0.46875</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -9601,7 +9689,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -9644,15 +9732,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="3"/>
@@ -9664,16 +9752,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>560</v>
+        <v>800</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -9730,7 +9818,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -9764,15 +9852,15 @@
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="P21" s="34">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>53.333333333333336</v>
       </c>
       <c r="Q21" s="34">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -9814,15 +9902,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>400</v>
+        <v>320</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -9864,15 +9952,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -9905,7 +9993,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9930,7 +10018,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -9943,14 +10031,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="78">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="78">
         <f>'Project Summary'!N1</f>
@@ -9959,15 +10047,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -9976,29 +10064,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="22" customFormat="1">
       <c r="A5" s="22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="81" t="str">
@@ -10248,18 +10336,24 @@
       <c r="M10" s="14">
         <v>100</v>
       </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="N10" s="14">
+        <v>80</v>
+      </c>
+      <c r="O10" s="14">
+        <v>60</v>
+      </c>
+      <c r="P10" s="14">
+        <v>60</v>
+      </c>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="1"/>
-        <v>740</v>
+        <v>940</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="0"/>
-        <v>740</v>
+        <v>940</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -10288,18 +10382,24 @@
       <c r="M11" s="14">
         <v>28</v>
       </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="N11" s="14">
+        <v>48</v>
+      </c>
+      <c r="O11" s="14">
+        <v>68</v>
+      </c>
+      <c r="P11" s="14">
+        <v>68</v>
+      </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>212</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="56">
@@ -10535,7 +10635,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -10578,15 +10678,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="3"/>
@@ -10598,11 +10698,11 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="1"/>
-        <v>896</v>
+        <v>1280</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="2"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
@@ -10661,7 +10761,7 @@
     </row>
     <row r="20" spans="1:21" hidden="1">
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1">
         <v>960</v>
@@ -10843,7 +10943,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -10868,7 +10968,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -10881,14 +10981,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -10897,15 +10997,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -10914,29 +11014,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -11071,18 +11171,24 @@
       <c r="M7" s="3">
         <v>4</v>
       </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
+      <c r="N7" s="3">
+        <v>4</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3">
+        <v>4</v>
+      </c>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -11314,18 +11420,24 @@
       <c r="M13" s="3">
         <v>4</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="N13" s="3">
+        <v>4</v>
+      </c>
+      <c r="O13" s="3">
+        <v>4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4</v>
+      </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -11482,7 +11594,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -11525,15 +11637,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -11545,16 +11657,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -11611,7 +11723,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:21" hidden="1">
@@ -11645,15 +11757,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -11695,15 +11807,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -11745,15 +11857,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -11786,7 +11898,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -11811,7 +11923,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -11824,14 +11936,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -11840,15 +11952,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -11858,29 +11970,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12211,18 +12323,24 @@
       <c r="M12" s="14">
         <v>160</v>
       </c>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
+      <c r="N12" s="14">
+        <v>160</v>
+      </c>
+      <c r="O12" s="14">
+        <v>160</v>
+      </c>
+      <c r="P12" s="14">
+        <v>160</v>
+      </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
       <c r="T12" s="6">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>720</v>
       </c>
       <c r="U12" s="26">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>720</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -12417,7 +12535,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -12460,15 +12578,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -12480,16 +12598,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1600</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -12546,7 +12664,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -12583,15 +12701,15 @@
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="P21" s="34">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>106.66666666666667</v>
       </c>
       <c r="Q21" s="34">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -12633,15 +12751,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>800</v>
+        <v>640</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -12683,15 +12801,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -12724,7 +12842,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12749,7 +12867,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -12762,14 +12880,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -12778,15 +12896,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -12795,29 +12913,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -12952,18 +13070,24 @@
       <c r="M7" s="14">
         <v>20</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="N7" s="14">
+        <v>20</v>
+      </c>
+      <c r="O7" s="14">
+        <v>20</v>
+      </c>
+      <c r="P7" s="14">
+        <v>20</v>
+      </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="14"/>
       <c r="T7" s="6">
         <f t="shared" ref="T7:T18" si="0">SUM(G7:R7)</f>
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="U7" s="26">
         <f>T7/MAX(C7,1)</f>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -13195,18 +13319,24 @@
       <c r="M13" s="14">
         <v>20</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
+      <c r="N13" s="14">
+        <v>20</v>
+      </c>
+      <c r="O13" s="14">
+        <v>20</v>
+      </c>
+      <c r="P13" s="14">
+        <v>20</v>
+      </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>197</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>0.68500000000000005</v>
+        <v>0.98499999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -13365,7 +13495,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -13408,15 +13538,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -13428,16 +13558,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>277</v>
+        <v>397</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.57708333333333328</v>
+        <v>0.82708333333333328</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -13494,7 +13624,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -13531,15 +13661,15 @@
       </c>
       <c r="N21" s="34">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>50.75</v>
+        <v>40.75</v>
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>30.75</v>
       </c>
       <c r="P21" s="34">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>27.666666666666668</v>
       </c>
       <c r="Q21" s="34">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -13581,15 +13711,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -13631,15 +13761,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -13672,10 +13802,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -13700,7 +13833,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -13713,14 +13846,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -13729,15 +13862,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -13746,29 +13879,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:21" s="47" customFormat="1">
       <c r="A5" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -14208,18 +14341,24 @@
       <c r="M15" s="14">
         <v>16</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="N15" s="14">
+        <v>16</v>
+      </c>
+      <c r="O15" s="14">
+        <v>16</v>
+      </c>
+      <c r="P15" s="14">
+        <v>16</v>
+      </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="T15" s="6">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="U15" s="26">
         <f t="shared" si="1"/>
-        <v>0.73684210526315785</v>
+        <v>1.0526315789473684</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -14298,23 +14437,29 @@
       <c r="M17" s="14">
         <v>16</v>
       </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
+      <c r="N17" s="14">
+        <v>16</v>
+      </c>
+      <c r="O17" s="14">
+        <v>16</v>
+      </c>
+      <c r="P17" s="14">
+        <v>16</v>
+      </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
       <c r="T17" s="6">
         <f t="shared" si="0"/>
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="U17" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -14386,7 +14531,7 @@
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -14443,7 +14588,7 @@
     </row>
     <row r="20" spans="1:21" s="31" customFormat="1" hidden="1">
       <c r="B20" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="32">
         <v>288</v>
@@ -14484,11 +14629,11 @@
       </c>
       <c r="O21" s="34">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="P21" s="34">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="Q21" s="34">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -14534,11 +14679,11 @@
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -14580,15 +14725,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -14608,9 +14753,10 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
@@ -14621,8 +14767,8 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="20120" topLeftCell="V1"/>
-      <selection activeCell="M14" sqref="M14"/>
+      <pane xSplit="25380" topLeftCell="V1"/>
+      <selection activeCell="Q13" sqref="Q13"/>
       <selection pane="topRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -14648,7 +14794,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -14661,14 +14807,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -14677,15 +14823,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -14695,29 +14841,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="15" customFormat="1">
       <c r="A5" s="15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="81" t="str">
         <f>'Project Summary'!G3</f>
@@ -15002,18 +15148,24 @@
       <c r="M11" s="14">
         <v>80</v>
       </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="N11" s="14">
+        <v>80</v>
+      </c>
+      <c r="O11" s="14">
+        <v>80</v>
+      </c>
+      <c r="P11" s="14">
+        <v>80</v>
+      </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
       <c r="T11" s="6">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>560</v>
       </c>
       <c r="U11" s="26">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="42">
@@ -15092,18 +15244,24 @@
       <c r="M13" s="14">
         <v>80</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
+      <c r="N13" s="14">
+        <v>80</v>
+      </c>
+      <c r="O13" s="14">
+        <v>80</v>
+      </c>
+      <c r="P13" s="14">
+        <v>80</v>
+      </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="14"/>
       <c r="T13" s="6">
         <f t="shared" si="0"/>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="U13" s="26">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="42">
@@ -15260,7 +15418,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -15303,15 +15461,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -15323,16 +15481,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1600</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -15389,7 +15547,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -15397,7 +15555,7 @@
     </row>
     <row r="21" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" s="6">
         <f>IF(G23 = 0, 0, (C18-SUM(G18:G18))/(MONTH(N1-G5)))</f>
@@ -15429,15 +15587,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>106.66666666666667</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -15450,7 +15608,7 @@
     </row>
     <row r="22" spans="1:21" hidden="1">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G22" s="6">
         <f>IF(G23=0, 0, C18-SUM(G18:G18))</f>
@@ -15482,15 +15640,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>800</v>
+        <v>640</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -15503,7 +15661,7 @@
     </row>
     <row r="23" spans="1:21" hidden="1">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G23" s="6">
         <f>'Project Summary'!G16</f>
@@ -15535,15 +15693,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>
@@ -15576,7 +15734,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15601,7 +15759,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="94" t="str">
@@ -15614,14 +15772,14 @@
       <c r="G1" s="94"/>
       <c r="H1" s="94"/>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L1" s="82">
         <f>'Project Summary'!L1</f>
         <v>39980</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="82">
         <f>'Project Summary'!N1</f>
@@ -15630,15 +15788,15 @@
     </row>
     <row r="2" spans="1:21">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="G2" s="94" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="26">
@@ -15647,29 +15805,29 @@
     </row>
     <row r="3" spans="1:21">
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
     <row r="5" spans="1:21" s="20" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="81" t="str">
@@ -15921,18 +16079,24 @@
       <c r="M10" s="14">
         <v>160</v>
       </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="N10" s="14">
+        <v>160</v>
+      </c>
+      <c r="O10" s="14">
+        <v>160</v>
+      </c>
+      <c r="P10" s="14">
+        <v>160</v>
+      </c>
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
       <c r="T10" s="6">
         <f t="shared" si="0"/>
-        <v>960</v>
+        <v>1440</v>
       </c>
       <c r="U10" s="26">
         <f t="shared" si="1"/>
-        <v>960</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -16203,7 +16367,7 @@
     </row>
     <row r="18" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A18" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -16246,15 +16410,15 @@
       </c>
       <c r="N18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="O18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P18" s="25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="Q18" s="25">
         <f t="shared" si="2"/>
@@ -16266,16 +16430,16 @@
       </c>
       <c r="T18" s="6">
         <f t="shared" si="0"/>
-        <v>1120</v>
+        <v>1600</v>
       </c>
       <c r="U18" s="26">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:21" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="26">
         <f xml:space="preserve"> IF(C18&lt;T18, (T18-C18)/MAX(C18,1),0 )</f>
@@ -16332,7 +16496,7 @@
     </row>
     <row r="20" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="B20" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6">
         <v>1920</v>
@@ -16369,15 +16533,15 @@
       </c>
       <c r="N21" s="6">
         <f>IF(N23 = 0, 0, (C18-SUM(G18:N18))/(MONTH(N1-N5)))</f>
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="O21" s="6">
         <f>IF(O23 = 0, 0, (C18-SUM(G18:O18))/(MONTH(N1-O5)))</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="P21" s="6">
         <f>IF(P23 = 0, 0, (C18-SUM(G18:P18))/(MONTH(N1-P5)))</f>
-        <v>0</v>
+        <v>106.66666666666667</v>
       </c>
       <c r="Q21" s="6">
         <f>IF(Q23 = 0, 0, (C18-SUM(G18:Q18))/(MONTH(N1-Q5)))</f>
@@ -16419,15 +16583,15 @@
       </c>
       <c r="N22" s="6">
         <f>IF(N23=0, 0,C18-SUM(G18:N18))</f>
-        <v>800</v>
+        <v>640</v>
       </c>
       <c r="O22" s="6">
         <f>IF(O23=0, 0,C18-SUM(G18:O18))</f>
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="P22" s="6">
         <f>IF(P23=0, 0,C18-SUM(G18:P18))</f>
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="Q22" s="6">
         <f>IF(Q23=0, 0,C18-SUM(G18:Q18))</f>
@@ -16469,15 +16633,15 @@
       </c>
       <c r="N23" s="6">
         <f>'Project Summary'!N16</f>
-        <v>8</v>
+        <v>788</v>
       </c>
       <c r="O23" s="6">
         <f>'Project Summary'!O16</f>
-        <v>0</v>
+        <v>708</v>
       </c>
       <c r="P23" s="6">
         <f>'Project Summary'!P16</f>
-        <v>0</v>
+        <v>788</v>
       </c>
       <c r="Q23" s="6">
         <f>'Project Summary'!Q16</f>

</xml_diff>